<commit_message>
support binary balance tree
</commit_message>
<xml_diff>
--- a/EDA_database_algorithm.xlsx
+++ b/EDA_database_algorithm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PCNL\人才培养\计划\标准库建设\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\respo\iEDA-standard-develop-codebase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723B6369-1A40-4739-A6B3-AF6BA9DFDE5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84F7097-E950-4100-94B4-D67ED5109D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{5A250FBF-FD77-48BD-871A-3834DD962A5A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{5A250FBF-FD77-48BD-871A-3834DD962A5A}"/>
   </bookViews>
   <sheets>
     <sheet name="数据结构" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="233">
   <si>
     <t>EDA数据结构</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -927,6 +927,29 @@
   </si>
   <si>
     <t>TBD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李英奇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一般</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>见文档</t>
+  </si>
+  <si>
+    <t>见文档</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -985,7 +1008,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -995,6 +1018,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1067,7 +1096,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1086,9 +1115,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1101,6 +1127,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1110,8 +1142,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1431,18 +1466,18 @@
   <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.08203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.9296875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="8.19921875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.53125" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="9.06640625" style="5"/>
+    <col min="1" max="1" width="15.9140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="9.08203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1468,14 +1503,14 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>5</v>
+        <v>227</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:10" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="3"/>
@@ -1490,11 +1525,11 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="11" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1508,9 +1543,9 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+    <row r="4" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1522,9 +1557,9 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+    <row r="5" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1536,9 +1571,9 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6" t="s">
+    <row r="6" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1552,9 +1587,9 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
+    <row r="7" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
@@ -1566,23 +1601,35 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="4" t="s">
+    <row r="8" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
+      <c r="D8" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="I8" s="16">
+        <v>44483</v>
+      </c>
+      <c r="J8" s="15"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
@@ -1594,9 +1641,9 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+    <row r="10" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
@@ -1608,9 +1655,9 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+    <row r="11" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="4" t="s">
         <v>40</v>
       </c>
@@ -1622,9 +1669,9 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
+    <row r="12" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="4" t="s">
         <v>41</v>
       </c>
@@ -1636,9 +1683,9 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+    <row r="13" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="4" t="s">
         <v>18</v>
       </c>
@@ -1650,12 +1697,12 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6" t="s">
+    <row r="14" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="4"/>
@@ -1666,9 +1713,9 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
+    <row r="15" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
@@ -1680,10 +1727,10 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10" ht="15.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7" t="s">
+    <row r="16" spans="1:10" ht="15.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="6" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="4"/>
@@ -1694,10 +1741,10 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7" t="s">
+    <row r="17" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="4"/>
@@ -1708,10 +1755,10 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7" t="s">
+    <row r="18" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D18" s="4"/>
@@ -1722,10 +1769,10 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7" t="s">
+    <row r="19" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="4"/>
@@ -1736,10 +1783,10 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7" t="s">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D20" s="4"/>
@@ -1750,10 +1797,10 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7" t="s">
+    <row r="21" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="4"/>
@@ -1764,12 +1811,12 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6" t="s">
+    <row r="22" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>32</v>
       </c>
       <c r="D22" s="4"/>
@@ -1780,10 +1827,10 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7" t="s">
+    <row r="23" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="4"/>
@@ -1794,10 +1841,10 @@
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7" t="s">
+    <row r="24" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D24" s="4"/>
@@ -1808,10 +1855,10 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7" t="s">
+    <row r="25" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D25" s="4"/>
@@ -1822,10 +1869,10 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="7" t="s">
+    <row r="26" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D26" s="4"/>
@@ -1836,10 +1883,10 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7" t="s">
+    <row r="27" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D27" s="4"/>
@@ -1850,10 +1897,10 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:10" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7" t="s">
+    <row r="28" spans="1:10" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D28" s="4"/>
@@ -1864,10 +1911,10 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="7" t="s">
+    <row r="29" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D29" s="4"/>
@@ -1878,10 +1925,10 @@
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="7" t="s">
+    <row r="30" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D30" s="4"/>
@@ -1892,10 +1939,10 @@
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7" t="s">
+    <row r="31" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D31" s="4"/>
@@ -1906,10 +1953,10 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="7" t="s">
+    <row r="32" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="6" t="s">
         <v>120</v>
       </c>
       <c r="D32" s="4"/>
@@ -1920,10 +1967,10 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="7" t="s">
+    <row r="33" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D33" s="4"/>
@@ -1934,12 +1981,12 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6" t="s">
+    <row r="34" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="6" t="s">
         <v>50</v>
       </c>
       <c r="D34" s="4"/>
@@ -1950,10 +1997,10 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="7" t="s">
+    <row r="35" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="6" t="s">
         <v>48</v>
       </c>
       <c r="D35" s="4"/>
@@ -1964,10 +2011,10 @@
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
     </row>
-    <row r="36" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="7" t="s">
+    <row r="36" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D36" s="4"/>
@@ -1978,10 +2025,10 @@
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="7" t="s">
+    <row r="37" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D37" s="4"/>
@@ -1992,10 +2039,10 @@
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
     </row>
-    <row r="38" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="7" t="s">
+    <row r="38" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D38" s="4"/>
@@ -2006,14 +2053,14 @@
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
     </row>
-    <row r="39" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="6" t="s">
+    <row r="39" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D39" s="4"/>
@@ -2024,12 +2071,12 @@
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
     </row>
-    <row r="40" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6" t="s">
+    <row r="40" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="11"/>
+      <c r="B40" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="6" t="s">
         <v>53</v>
       </c>
       <c r="D40" s="4"/>
@@ -2040,10 +2087,10 @@
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="7" t="s">
+    <row r="41" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="6" t="s">
         <v>62</v>
       </c>
       <c r="D41" s="4"/>
@@ -2054,10 +2101,10 @@
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
     </row>
-    <row r="42" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="7" t="s">
+    <row r="42" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="6" t="s">
         <v>56</v>
       </c>
       <c r="D42" s="4"/>
@@ -2068,10 +2115,10 @@
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
     </row>
-    <row r="43" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="7" t="s">
+    <row r="43" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="6" t="s">
         <v>65</v>
       </c>
       <c r="D43" s="4"/>
@@ -2082,10 +2129,10 @@
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
     </row>
-    <row r="44" spans="1:10" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="7" t="s">
+    <row r="44" spans="1:10" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="6" t="s">
         <v>66</v>
       </c>
       <c r="D44" s="4"/>
@@ -2096,10 +2143,10 @@
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
     </row>
-    <row r="45" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="7" t="s">
+    <row r="45" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D45" s="4"/>
@@ -2110,12 +2157,12 @@
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
     </row>
-    <row r="46" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6" t="s">
+    <row r="46" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="11"/>
+      <c r="B46" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="6" t="s">
         <v>58</v>
       </c>
       <c r="D46" s="4"/>
@@ -2126,10 +2173,10 @@
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
     </row>
-    <row r="47" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="7" t="s">
+    <row r="47" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="11"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D47" s="4"/>
@@ -2140,10 +2187,10 @@
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
     </row>
-    <row r="48" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="7" t="s">
+    <row r="48" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="11"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="6" t="s">
         <v>60</v>
       </c>
       <c r="D48" s="4"/>
@@ -2154,10 +2201,10 @@
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
     </row>
-    <row r="49" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="7" t="s">
+    <row r="49" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="11"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="6" t="s">
         <v>61</v>
       </c>
       <c r="D49" s="4"/>
@@ -2168,10 +2215,10 @@
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
     </row>
-    <row r="50" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="7" t="s">
+    <row r="50" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="11"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="6" t="s">
         <v>64</v>
       </c>
       <c r="D50" s="4"/>
@@ -2182,10 +2229,10 @@
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
     </row>
-    <row r="51" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="7" t="s">
+    <row r="51" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="6" t="s">
         <v>68</v>
       </c>
       <c r="D51" s="4"/>
@@ -2196,7 +2243,7 @@
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
     </row>
-    <row r="52" spans="1:10" ht="14.25" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="52" spans="1:10" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A39:A51"/>
@@ -2219,20 +2266,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1B1B9C-0591-4BED-8FBD-040911B92B66}">
   <dimension ref="A1:J150"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.06640625" customWidth="1"/>
-    <col min="2" max="2" width="10.796875" customWidth="1"/>
+    <col min="1" max="1" width="11.08203125" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.9296875" customWidth="1"/>
-    <col min="5" max="5" width="12.86328125" customWidth="1"/>
+    <col min="4" max="4" width="11.9140625" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2264,11 +2311,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="11" t="s">
         <v>73</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -2284,9 +2331,9 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
+    <row r="3" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="4" t="s">
         <v>75</v>
       </c>
@@ -2300,9 +2347,9 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+    <row r="4" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="4" t="s">
         <v>77</v>
       </c>
@@ -2316,9 +2363,9 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+    <row r="5" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="4" t="s">
         <v>79</v>
       </c>
@@ -2332,9 +2379,9 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
+    <row r="6" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="4" t="s">
         <v>78</v>
       </c>
@@ -2348,9 +2395,9 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
+    <row r="7" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="4" t="s">
         <v>80</v>
       </c>
@@ -2364,9 +2411,9 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
+    <row r="8" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="4" t="s">
         <v>81</v>
       </c>
@@ -2382,9 +2429,9 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
+    <row r="9" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="4" t="s">
         <v>84</v>
       </c>
@@ -2398,9 +2445,9 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6" t="s">
+    <row r="10" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11" t="s">
         <v>85</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -2414,9 +2461,9 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+    <row r="11" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="4" t="s">
         <v>87</v>
       </c>
@@ -2428,9 +2475,9 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
+    <row r="12" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="4" t="s">
         <v>88</v>
       </c>
@@ -2442,10 +2489,10 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" ht="14.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7" t="s">
+    <row r="13" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="6" t="s">
         <v>89</v>
       </c>
       <c r="D13" s="4"/>
@@ -2458,9 +2505,9 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
+    <row r="14" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="4" t="s">
         <v>90</v>
       </c>
@@ -2472,10 +2519,10 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7" t="s">
+    <row r="15" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="6" t="s">
         <v>91</v>
       </c>
       <c r="D15" s="4"/>
@@ -2486,12 +2533,12 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6" t="s">
+    <row r="16" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>102</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -2506,10 +2553,10 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7" t="s">
+    <row r="17" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="6" t="s">
         <v>94</v>
       </c>
       <c r="D17" s="4"/>
@@ -2522,10 +2569,10 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="14" t="s">
+    <row r="18" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="10" t="s">
         <v>96</v>
       </c>
       <c r="D18" s="4"/>
@@ -2538,10 +2585,10 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7" t="s">
+    <row r="19" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="6" t="s">
         <v>98</v>
       </c>
       <c r="D19" s="4"/>
@@ -2554,10 +2601,10 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7" t="s">
+    <row r="20" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="6" t="s">
         <v>100</v>
       </c>
       <c r="D20" s="4"/>
@@ -2570,10 +2617,10 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7" t="s">
+    <row r="21" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="6" t="s">
         <v>101</v>
       </c>
       <c r="D21" s="4"/>
@@ -2586,12 +2633,12 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6" t="s">
+    <row r="22" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>104</v>
       </c>
       <c r="D22" s="4"/>
@@ -2602,10 +2649,10 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7" t="s">
+    <row r="23" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="6" t="s">
         <v>105</v>
       </c>
       <c r="D23" s="4"/>
@@ -2616,10 +2663,10 @@
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7" t="s">
+    <row r="24" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="6" t="s">
         <v>106</v>
       </c>
       <c r="D24" s="4"/>
@@ -2630,10 +2677,10 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7" t="s">
+    <row r="25" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="6" t="s">
         <v>107</v>
       </c>
       <c r="D25" s="4"/>
@@ -2644,10 +2691,10 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="7" t="s">
+    <row r="26" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="6" t="s">
         <v>108</v>
       </c>
       <c r="D26" s="4"/>
@@ -2658,12 +2705,12 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6" t="s">
+    <row r="27" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>109</v>
       </c>
       <c r="D27" s="4"/>
@@ -2674,10 +2721,10 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7" t="s">
+    <row r="28" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="6" t="s">
         <v>110</v>
       </c>
       <c r="D28" s="4"/>
@@ -2688,10 +2735,10 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="7" t="s">
+    <row r="29" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="6" t="s">
         <v>111</v>
       </c>
       <c r="D29" s="4"/>
@@ -2702,10 +2749,10 @@
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="7" t="s">
+    <row r="30" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="6" t="s">
         <v>112</v>
       </c>
       <c r="D30" s="4"/>
@@ -2716,10 +2763,10 @@
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7" t="s">
+    <row r="31" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="6" t="s">
         <v>139</v>
       </c>
       <c r="D31" s="4"/>
@@ -2730,10 +2777,10 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="7" t="s">
+    <row r="32" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="6" t="s">
         <v>113</v>
       </c>
       <c r="D32" s="4"/>
@@ -2744,10 +2791,10 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="7" t="s">
+    <row r="33" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="6" t="s">
         <v>114</v>
       </c>
       <c r="D33" s="4"/>
@@ -2758,10 +2805,10 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="7" t="s">
+    <row r="34" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="6" t="s">
         <v>115</v>
       </c>
       <c r="D34" s="4"/>
@@ -2772,10 +2819,10 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="7" t="s">
+    <row r="35" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="6" t="s">
         <v>116</v>
       </c>
       <c r="D35" s="4"/>
@@ -2786,10 +2833,10 @@
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
     </row>
-    <row r="36" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="7" t="s">
+    <row r="36" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="6" t="s">
         <v>122</v>
       </c>
       <c r="D36" s="4"/>
@@ -2800,10 +2847,10 @@
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="7" t="s">
+    <row r="37" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="6" t="s">
         <v>123</v>
       </c>
       <c r="D37" s="4"/>
@@ -2814,10 +2861,10 @@
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
     </row>
-    <row r="38" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="7" t="s">
+    <row r="38" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="6" t="s">
         <v>118</v>
       </c>
       <c r="D38" s="4"/>
@@ -2828,10 +2875,10 @@
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
     </row>
-    <row r="39" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="7" t="s">
+    <row r="39" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="6" t="s">
         <v>117</v>
       </c>
       <c r="D39" s="4"/>
@@ -2842,10 +2889,10 @@
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
     </row>
-    <row r="40" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="7" t="s">
+    <row r="40" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="6" t="s">
         <v>119</v>
       </c>
       <c r="D40" s="4"/>
@@ -2856,10 +2903,10 @@
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="7" t="s">
+    <row r="41" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="6" t="s">
         <v>121</v>
       </c>
       <c r="D41" s="4"/>
@@ -2870,10 +2917,10 @@
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
     </row>
-    <row r="42" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="7" t="s">
+    <row r="42" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="6" t="s">
         <v>124</v>
       </c>
       <c r="D42" s="4"/>
@@ -2884,10 +2931,10 @@
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
     </row>
-    <row r="43" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="7" t="s">
+    <row r="43" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="6" t="s">
         <v>125</v>
       </c>
       <c r="D43" s="4"/>
@@ -2898,10 +2945,10 @@
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
     </row>
-    <row r="44" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="7" t="s">
+    <row r="44" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D44" s="4"/>
@@ -2912,10 +2959,10 @@
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
     </row>
-    <row r="45" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="7" t="s">
+    <row r="45" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="6" t="s">
         <v>127</v>
       </c>
       <c r="D45" s="4"/>
@@ -2926,10 +2973,10 @@
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
     </row>
-    <row r="46" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="7" t="s">
+    <row r="46" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="6" t="s">
         <v>128</v>
       </c>
       <c r="D46" s="4"/>
@@ -2940,10 +2987,10 @@
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
     </row>
-    <row r="47" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="7" t="s">
+    <row r="47" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="11"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="6" t="s">
         <v>129</v>
       </c>
       <c r="D47" s="4"/>
@@ -2954,10 +3001,10 @@
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
     </row>
-    <row r="48" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="7" t="s">
+    <row r="48" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="11"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="6" t="s">
         <v>132</v>
       </c>
       <c r="D48" s="4"/>
@@ -2968,10 +3015,10 @@
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
     </row>
-    <row r="49" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="7" t="s">
+    <row r="49" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="11"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="6" t="s">
         <v>130</v>
       </c>
       <c r="D49" s="4"/>
@@ -2982,10 +3029,10 @@
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
     </row>
-    <row r="50" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="7" t="s">
+    <row r="50" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="11"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="6" t="s">
         <v>131</v>
       </c>
       <c r="D50" s="4"/>
@@ -2996,10 +3043,10 @@
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
     </row>
-    <row r="51" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="7" t="s">
+    <row r="51" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D51" s="4"/>
@@ -3010,10 +3057,10 @@
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
     </row>
-    <row r="52" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="7" t="s">
+    <row r="52" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="11"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="6" t="s">
         <v>134</v>
       </c>
       <c r="D52" s="4"/>
@@ -3024,10 +3071,10 @@
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
     </row>
-    <row r="53" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="7" t="s">
+    <row r="53" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="11"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="6" t="s">
         <v>136</v>
       </c>
       <c r="D53" s="4"/>
@@ -3038,10 +3085,10 @@
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
     </row>
-    <row r="54" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="7" t="s">
+    <row r="54" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="11"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="6" t="s">
         <v>137</v>
       </c>
       <c r="D54" s="4"/>
@@ -3052,10 +3099,10 @@
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
     </row>
-    <row r="55" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="6"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="7" t="s">
+    <row r="55" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="11"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="6" t="s">
         <v>138</v>
       </c>
       <c r="D55" s="4"/>
@@ -3066,10 +3113,10 @@
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
     </row>
-    <row r="56" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="7" t="s">
+    <row r="56" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="11"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="6" t="s">
         <v>178</v>
       </c>
       <c r="D56" s="4"/>
@@ -3080,10 +3127,10 @@
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
     </row>
-    <row r="57" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="6"/>
-      <c r="B57" s="6"/>
-      <c r="C57" s="7" t="s">
+    <row r="57" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="11"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="6" t="s">
         <v>177</v>
       </c>
       <c r="D57" s="4"/>
@@ -3094,10 +3141,10 @@
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
     </row>
-    <row r="58" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="6"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="7" t="s">
+    <row r="58" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="11"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="6" t="s">
         <v>135</v>
       </c>
       <c r="D58" s="4"/>
@@ -3108,12 +3155,12 @@
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
     </row>
-    <row r="59" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="6"/>
-      <c r="B59" s="6" t="s">
+    <row r="59" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="11"/>
+      <c r="B59" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="6" t="s">
         <v>93</v>
       </c>
       <c r="D59" s="4"/>
@@ -3126,10 +3173,10 @@
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
     </row>
-    <row r="60" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="6"/>
-      <c r="B60" s="6"/>
-      <c r="C60" s="7" t="s">
+    <row r="60" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="11"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D60" s="4"/>
@@ -3142,10 +3189,10 @@
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
     </row>
-    <row r="61" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="6"/>
-      <c r="B61" s="6"/>
-      <c r="C61" s="7" t="s">
+    <row r="61" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="11"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="6" t="s">
         <v>140</v>
       </c>
       <c r="D61" s="4"/>
@@ -3156,10 +3203,10 @@
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
     </row>
-    <row r="62" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="6"/>
-      <c r="B62" s="6"/>
-      <c r="C62" s="7" t="s">
+    <row r="62" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="11"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="6" t="s">
         <v>141</v>
       </c>
       <c r="D62" s="4"/>
@@ -3170,10 +3217,10 @@
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
     </row>
-    <row r="63" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="6"/>
-      <c r="B63" s="6"/>
-      <c r="C63" s="7" t="s">
+    <row r="63" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="11"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="6" t="s">
         <v>142</v>
       </c>
       <c r="D63" s="4"/>
@@ -3184,10 +3231,10 @@
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
     </row>
-    <row r="64" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="6"/>
-      <c r="B64" s="6"/>
-      <c r="C64" s="7" t="s">
+    <row r="64" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="11"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="6" t="s">
         <v>143</v>
       </c>
       <c r="D64" s="4"/>
@@ -3198,10 +3245,10 @@
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
     </row>
-    <row r="65" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="6"/>
-      <c r="B65" s="6"/>
-      <c r="C65" s="7" t="s">
+    <row r="65" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="11"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="6" t="s">
         <v>144</v>
       </c>
       <c r="D65" s="4"/>
@@ -3212,10 +3259,10 @@
       <c r="I65" s="4"/>
       <c r="J65" s="4"/>
     </row>
-    <row r="66" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="6"/>
-      <c r="B66" s="6"/>
-      <c r="C66" s="7" t="s">
+    <row r="66" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="11"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="6" t="s">
         <v>145</v>
       </c>
       <c r="D66" s="4"/>
@@ -3226,10 +3273,10 @@
       <c r="I66" s="4"/>
       <c r="J66" s="4"/>
     </row>
-    <row r="67" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="6"/>
-      <c r="B67" s="6"/>
-      <c r="C67" s="7" t="s">
+    <row r="67" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="11"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="6" t="s">
         <v>146</v>
       </c>
       <c r="D67" s="4"/>
@@ -3240,10 +3287,10 @@
       <c r="I67" s="4"/>
       <c r="J67" s="4"/>
     </row>
-    <row r="68" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A68" s="6"/>
-      <c r="B68" s="6"/>
-      <c r="C68" s="7" t="s">
+    <row r="68" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="11"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="6" t="s">
         <v>149</v>
       </c>
       <c r="D68" s="4"/>
@@ -3254,10 +3301,10 @@
       <c r="I68" s="4"/>
       <c r="J68" s="4"/>
     </row>
-    <row r="69" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="6"/>
-      <c r="B69" s="6"/>
-      <c r="C69" s="7" t="s">
+    <row r="69" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="11"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="6" t="s">
         <v>150</v>
       </c>
       <c r="D69" s="4"/>
@@ -3268,12 +3315,12 @@
       <c r="I69" s="4"/>
       <c r="J69" s="4"/>
     </row>
-    <row r="70" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="6"/>
-      <c r="B70" s="6" t="s">
+    <row r="70" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="11"/>
+      <c r="B70" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C70" s="6" t="s">
         <v>151</v>
       </c>
       <c r="D70" s="4"/>
@@ -3284,10 +3331,10 @@
       <c r="I70" s="4"/>
       <c r="J70" s="4"/>
     </row>
-    <row r="71" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A71" s="6"/>
-      <c r="B71" s="6"/>
-      <c r="C71" s="7" t="s">
+    <row r="71" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="11"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="6" t="s">
         <v>153</v>
       </c>
       <c r="D71" s="4"/>
@@ -3298,10 +3345,10 @@
       <c r="I71" s="4"/>
       <c r="J71" s="4"/>
     </row>
-    <row r="72" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="6"/>
-      <c r="B72" s="6"/>
-      <c r="C72" s="7" t="s">
+    <row r="72" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="11"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="6" t="s">
         <v>154</v>
       </c>
       <c r="D72" s="4"/>
@@ -3312,10 +3359,10 @@
       <c r="I72" s="4"/>
       <c r="J72" s="4"/>
     </row>
-    <row r="73" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A73" s="6"/>
-      <c r="B73" s="6"/>
-      <c r="C73" s="7" t="s">
+    <row r="73" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="11"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="6" t="s">
         <v>155</v>
       </c>
       <c r="D73" s="4"/>
@@ -3326,10 +3373,10 @@
       <c r="I73" s="4"/>
       <c r="J73" s="4"/>
     </row>
-    <row r="74" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A74" s="6"/>
-      <c r="B74" s="6"/>
-      <c r="C74" s="7" t="s">
+    <row r="74" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="11"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="6" t="s">
         <v>181</v>
       </c>
       <c r="D74" s="4"/>
@@ -3340,10 +3387,10 @@
       <c r="I74" s="4"/>
       <c r="J74" s="4"/>
     </row>
-    <row r="75" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A75" s="6"/>
-      <c r="B75" s="6"/>
-      <c r="C75" s="7" t="s">
+    <row r="75" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="11"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="6" t="s">
         <v>180</v>
       </c>
       <c r="D75" s="4"/>
@@ -3354,10 +3401,10 @@
       <c r="I75" s="4"/>
       <c r="J75" s="4"/>
     </row>
-    <row r="76" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A76" s="6"/>
-      <c r="B76" s="6"/>
-      <c r="C76" s="7" t="s">
+    <row r="76" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="11"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="6" t="s">
         <v>176</v>
       </c>
       <c r="D76" s="4"/>
@@ -3368,10 +3415,10 @@
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
     </row>
-    <row r="77" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A77" s="6"/>
-      <c r="B77" s="6"/>
-      <c r="C77" s="7" t="s">
+    <row r="77" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="11"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="6" t="s">
         <v>156</v>
       </c>
       <c r="D77" s="4"/>
@@ -3382,12 +3429,12 @@
       <c r="I77" s="4"/>
       <c r="J77" s="4"/>
     </row>
-    <row r="78" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A78" s="6"/>
-      <c r="B78" s="6" t="s">
+    <row r="78" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="11"/>
+      <c r="B78" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="C78" s="7" t="s">
+      <c r="C78" s="6" t="s">
         <v>158</v>
       </c>
       <c r="D78" s="4"/>
@@ -3398,10 +3445,10 @@
       <c r="I78" s="4"/>
       <c r="J78" s="4"/>
     </row>
-    <row r="79" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A79" s="6"/>
-      <c r="B79" s="6"/>
-      <c r="C79" s="7" t="s">
+    <row r="79" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="11"/>
+      <c r="B79" s="11"/>
+      <c r="C79" s="6" t="s">
         <v>159</v>
       </c>
       <c r="D79" s="4"/>
@@ -3412,10 +3459,10 @@
       <c r="I79" s="4"/>
       <c r="J79" s="4"/>
     </row>
-    <row r="80" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A80" s="6"/>
-      <c r="B80" s="6"/>
-      <c r="C80" s="7" t="s">
+    <row r="80" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="11"/>
+      <c r="B80" s="11"/>
+      <c r="C80" s="6" t="s">
         <v>160</v>
       </c>
       <c r="D80" s="4"/>
@@ -3426,10 +3473,10 @@
       <c r="I80" s="4"/>
       <c r="J80" s="4"/>
     </row>
-    <row r="81" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A81" s="6"/>
-      <c r="B81" s="6"/>
-      <c r="C81" s="7" t="s">
+    <row r="81" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="11"/>
+      <c r="B81" s="11"/>
+      <c r="C81" s="6" t="s">
         <v>161</v>
       </c>
       <c r="D81" s="4"/>
@@ -3440,10 +3487,10 @@
       <c r="I81" s="4"/>
       <c r="J81" s="4"/>
     </row>
-    <row r="82" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A82" s="6"/>
-      <c r="B82" s="6"/>
-      <c r="C82" s="7" t="s">
+    <row r="82" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="11"/>
+      <c r="B82" s="11"/>
+      <c r="C82" s="6" t="s">
         <v>162</v>
       </c>
       <c r="D82" s="4"/>
@@ -3454,12 +3501,12 @@
       <c r="I82" s="4"/>
       <c r="J82" s="4"/>
     </row>
-    <row r="83" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A83" s="6"/>
-      <c r="B83" s="6" t="s">
+    <row r="83" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="11"/>
+      <c r="B83" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="C83" s="7" t="s">
+      <c r="C83" s="6" t="s">
         <v>163</v>
       </c>
       <c r="D83" s="4"/>
@@ -3470,10 +3517,10 @@
       <c r="I83" s="4"/>
       <c r="J83" s="4"/>
     </row>
-    <row r="84" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A84" s="6"/>
-      <c r="B84" s="6"/>
-      <c r="C84" s="7" t="s">
+    <row r="84" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="11"/>
+      <c r="B84" s="11"/>
+      <c r="C84" s="6" t="s">
         <v>164</v>
       </c>
       <c r="D84" s="4"/>
@@ -3484,10 +3531,10 @@
       <c r="I84" s="4"/>
       <c r="J84" s="4"/>
     </row>
-    <row r="85" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A85" s="6"/>
-      <c r="B85" s="6"/>
-      <c r="C85" s="7" t="s">
+    <row r="85" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="11"/>
+      <c r="B85" s="11"/>
+      <c r="C85" s="6" t="s">
         <v>147</v>
       </c>
       <c r="D85" s="4"/>
@@ -3498,10 +3545,10 @@
       <c r="I85" s="4"/>
       <c r="J85" s="4"/>
     </row>
-    <row r="86" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A86" s="6"/>
-      <c r="B86" s="6"/>
-      <c r="C86" s="7" t="s">
+    <row r="86" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="11"/>
+      <c r="B86" s="11"/>
+      <c r="C86" s="6" t="s">
         <v>148</v>
       </c>
       <c r="D86" s="4"/>
@@ -3512,10 +3559,10 @@
       <c r="I86" s="4"/>
       <c r="J86" s="4"/>
     </row>
-    <row r="87" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A87" s="6"/>
-      <c r="B87" s="6"/>
-      <c r="C87" s="7" t="s">
+    <row r="87" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="11"/>
+      <c r="B87" s="11"/>
+      <c r="C87" s="6" t="s">
         <v>165</v>
       </c>
       <c r="D87" s="4"/>
@@ -3526,10 +3573,10 @@
       <c r="I87" s="4"/>
       <c r="J87" s="4"/>
     </row>
-    <row r="88" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A88" s="6"/>
-      <c r="B88" s="6"/>
-      <c r="C88" s="7" t="s">
+    <row r="88" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="11"/>
+      <c r="B88" s="11"/>
+      <c r="C88" s="6" t="s">
         <v>167</v>
       </c>
       <c r="D88" s="4"/>
@@ -3540,10 +3587,10 @@
       <c r="I88" s="4"/>
       <c r="J88" s="4"/>
     </row>
-    <row r="89" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A89" s="6"/>
-      <c r="B89" s="6"/>
-      <c r="C89" s="7" t="s">
+    <row r="89" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="11"/>
+      <c r="B89" s="11"/>
+      <c r="C89" s="6" t="s">
         <v>166</v>
       </c>
       <c r="D89" s="4"/>
@@ -3554,10 +3601,10 @@
       <c r="I89" s="4"/>
       <c r="J89" s="4"/>
     </row>
-    <row r="90" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A90" s="6"/>
-      <c r="B90" s="6"/>
-      <c r="C90" s="7" t="s">
+    <row r="90" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="11"/>
+      <c r="B90" s="11"/>
+      <c r="C90" s="6" t="s">
         <v>168</v>
       </c>
       <c r="D90" s="4"/>
@@ -3568,10 +3615,10 @@
       <c r="I90" s="4"/>
       <c r="J90" s="4"/>
     </row>
-    <row r="91" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A91" s="6"/>
-      <c r="B91" s="6"/>
-      <c r="C91" s="7" t="s">
+    <row r="91" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="11"/>
+      <c r="B91" s="11"/>
+      <c r="C91" s="6" t="s">
         <v>169</v>
       </c>
       <c r="D91" s="4"/>
@@ -3582,10 +3629,10 @@
       <c r="I91" s="4"/>
       <c r="J91" s="4"/>
     </row>
-    <row r="92" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A92" s="6"/>
-      <c r="B92" s="6"/>
-      <c r="C92" s="7" t="s">
+    <row r="92" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="11"/>
+      <c r="B92" s="11"/>
+      <c r="C92" s="6" t="s">
         <v>170</v>
       </c>
       <c r="D92" s="4"/>
@@ -3596,10 +3643,10 @@
       <c r="I92" s="4"/>
       <c r="J92" s="4"/>
     </row>
-    <row r="93" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A93" s="6"/>
-      <c r="B93" s="6"/>
-      <c r="C93" s="7" t="s">
+    <row r="93" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="11"/>
+      <c r="B93" s="11"/>
+      <c r="C93" s="6" t="s">
         <v>171</v>
       </c>
       <c r="D93" s="4"/>
@@ -3610,10 +3657,10 @@
       <c r="I93" s="4"/>
       <c r="J93" s="4"/>
     </row>
-    <row r="94" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A94" s="6"/>
-      <c r="B94" s="6"/>
-      <c r="C94" s="7" t="s">
+    <row r="94" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="11"/>
+      <c r="B94" s="11"/>
+      <c r="C94" s="6" t="s">
         <v>172</v>
       </c>
       <c r="D94" s="4"/>
@@ -3624,10 +3671,10 @@
       <c r="I94" s="4"/>
       <c r="J94" s="4"/>
     </row>
-    <row r="95" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A95" s="6"/>
-      <c r="B95" s="6"/>
-      <c r="C95" s="7" t="s">
+    <row r="95" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="11"/>
+      <c r="B95" s="11"/>
+      <c r="C95" s="6" t="s">
         <v>173</v>
       </c>
       <c r="D95" s="4"/>
@@ -3638,10 +3685,10 @@
       <c r="I95" s="4"/>
       <c r="J95" s="4"/>
     </row>
-    <row r="96" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A96" s="6"/>
-      <c r="B96" s="6"/>
-      <c r="C96" s="7" t="s">
+    <row r="96" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="11"/>
+      <c r="B96" s="11"/>
+      <c r="C96" s="6" t="s">
         <v>174</v>
       </c>
       <c r="D96" s="4"/>
@@ -3652,10 +3699,10 @@
       <c r="I96" s="4"/>
       <c r="J96" s="4"/>
     </row>
-    <row r="97" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A97" s="6"/>
-      <c r="B97" s="6"/>
-      <c r="C97" s="7" t="s">
+    <row r="97" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="11"/>
+      <c r="B97" s="11"/>
+      <c r="C97" s="6" t="s">
         <v>175</v>
       </c>
       <c r="D97" s="4"/>
@@ -3666,12 +3713,12 @@
       <c r="I97" s="4"/>
       <c r="J97" s="4"/>
     </row>
-    <row r="98" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A98" s="6"/>
-      <c r="B98" s="6" t="s">
+    <row r="98" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="11"/>
+      <c r="B98" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="C98" s="7" t="s">
+      <c r="C98" s="6" t="s">
         <v>90</v>
       </c>
       <c r="D98" s="4"/>
@@ -3682,10 +3729,10 @@
       <c r="I98" s="4"/>
       <c r="J98" s="4"/>
     </row>
-    <row r="99" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A99" s="6"/>
-      <c r="B99" s="6"/>
-      <c r="C99" s="7" t="s">
+    <row r="99" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="11"/>
+      <c r="B99" s="11"/>
+      <c r="C99" s="6" t="s">
         <v>182</v>
       </c>
       <c r="D99" s="4"/>
@@ -3696,10 +3743,10 @@
       <c r="I99" s="4"/>
       <c r="J99" s="4"/>
     </row>
-    <row r="100" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A100" s="6"/>
-      <c r="B100" s="6"/>
-      <c r="C100" s="7" t="s">
+    <row r="100" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="11"/>
+      <c r="B100" s="11"/>
+      <c r="C100" s="6" t="s">
         <v>183</v>
       </c>
       <c r="D100" s="4"/>
@@ -3710,10 +3757,10 @@
       <c r="I100" s="4"/>
       <c r="J100" s="4"/>
     </row>
-    <row r="101" spans="1:10" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A101" s="6"/>
-      <c r="B101" s="6"/>
-      <c r="C101" s="7" t="s">
+    <row r="101" spans="1:10" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="11"/>
+      <c r="B101" s="11"/>
+      <c r="C101" s="6" t="s">
         <v>184</v>
       </c>
       <c r="D101" s="4"/>
@@ -3724,10 +3771,10 @@
       <c r="I101" s="4"/>
       <c r="J101" s="4"/>
     </row>
-    <row r="102" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A102" s="6"/>
-      <c r="B102" s="6"/>
-      <c r="C102" s="7" t="s">
+    <row r="102" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="11"/>
+      <c r="B102" s="11"/>
+      <c r="C102" s="6" t="s">
         <v>185</v>
       </c>
       <c r="D102" s="4"/>
@@ -3738,10 +3785,10 @@
       <c r="I102" s="4"/>
       <c r="J102" s="4"/>
     </row>
-    <row r="103" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A103" s="6"/>
-      <c r="B103" s="6"/>
-      <c r="C103" s="7" t="s">
+    <row r="103" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="11"/>
+      <c r="B103" s="11"/>
+      <c r="C103" s="6" t="s">
         <v>186</v>
       </c>
       <c r="D103" s="4"/>
@@ -3752,10 +3799,10 @@
       <c r="I103" s="4"/>
       <c r="J103" s="4"/>
     </row>
-    <row r="104" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A104" s="6"/>
-      <c r="B104" s="6"/>
-      <c r="C104" s="7" t="s">
+    <row r="104" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="11"/>
+      <c r="B104" s="11"/>
+      <c r="C104" s="6" t="s">
         <v>187</v>
       </c>
       <c r="D104" s="4"/>
@@ -3766,10 +3813,10 @@
       <c r="I104" s="4"/>
       <c r="J104" s="4"/>
     </row>
-    <row r="105" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A105" s="6"/>
-      <c r="B105" s="6"/>
-      <c r="C105" s="7" t="s">
+    <row r="105" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="11"/>
+      <c r="B105" s="11"/>
+      <c r="C105" s="6" t="s">
         <v>188</v>
       </c>
       <c r="D105" s="4"/>
@@ -3780,10 +3827,10 @@
       <c r="I105" s="4"/>
       <c r="J105" s="4"/>
     </row>
-    <row r="106" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A106" s="6"/>
-      <c r="B106" s="6"/>
-      <c r="C106" s="7" t="s">
+    <row r="106" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A106" s="11"/>
+      <c r="B106" s="11"/>
+      <c r="C106" s="6" t="s">
         <v>189</v>
       </c>
       <c r="D106" s="4"/>
@@ -3794,10 +3841,10 @@
       <c r="I106" s="4"/>
       <c r="J106" s="4"/>
     </row>
-    <row r="107" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A107" s="6"/>
-      <c r="B107" s="6"/>
-      <c r="C107" s="7" t="s">
+    <row r="107" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A107" s="11"/>
+      <c r="B107" s="11"/>
+      <c r="C107" s="6" t="s">
         <v>190</v>
       </c>
       <c r="D107" s="4"/>
@@ -3808,10 +3855,10 @@
       <c r="I107" s="4"/>
       <c r="J107" s="4"/>
     </row>
-    <row r="108" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A108" s="6"/>
-      <c r="B108" s="6"/>
-      <c r="C108" s="7" t="s">
+    <row r="108" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="11"/>
+      <c r="B108" s="11"/>
+      <c r="C108" s="6" t="s">
         <v>191</v>
       </c>
       <c r="D108" s="4"/>
@@ -3822,10 +3869,10 @@
       <c r="I108" s="4"/>
       <c r="J108" s="4"/>
     </row>
-    <row r="109" spans="1:10" ht="18.399999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A109" s="6"/>
-      <c r="B109" s="6"/>
-      <c r="C109" s="7" t="s">
+    <row r="109" spans="1:10" ht="18.399999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="11"/>
+      <c r="B109" s="11"/>
+      <c r="C109" s="6" t="s">
         <v>192</v>
       </c>
       <c r="D109" s="4"/>
@@ -3836,10 +3883,10 @@
       <c r="I109" s="4"/>
       <c r="J109" s="4"/>
     </row>
-    <row r="110" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A110" s="6"/>
-      <c r="B110" s="6"/>
-      <c r="C110" s="7" t="s">
+    <row r="110" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="11"/>
+      <c r="B110" s="11"/>
+      <c r="C110" s="6" t="s">
         <v>193</v>
       </c>
       <c r="D110" s="4"/>
@@ -3850,10 +3897,10 @@
       <c r="I110" s="4"/>
       <c r="J110" s="4"/>
     </row>
-    <row r="111" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A111" s="6"/>
-      <c r="B111" s="6"/>
-      <c r="C111" s="7" t="s">
+    <row r="111" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="11"/>
+      <c r="B111" s="11"/>
+      <c r="C111" s="6" t="s">
         <v>194</v>
       </c>
       <c r="D111" s="4"/>
@@ -3864,10 +3911,10 @@
       <c r="I111" s="4"/>
       <c r="J111" s="4"/>
     </row>
-    <row r="112" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A112" s="6"/>
-      <c r="B112" s="6"/>
-      <c r="C112" s="7" t="s">
+    <row r="112" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="11"/>
+      <c r="B112" s="11"/>
+      <c r="C112" s="6" t="s">
         <v>195</v>
       </c>
       <c r="D112" s="4"/>
@@ -3878,10 +3925,10 @@
       <c r="I112" s="4"/>
       <c r="J112" s="4"/>
     </row>
-    <row r="113" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A113" s="6"/>
-      <c r="B113" s="6"/>
-      <c r="C113" s="7" t="s">
+    <row r="113" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="11"/>
+      <c r="B113" s="11"/>
+      <c r="C113" s="6" t="s">
         <v>196</v>
       </c>
       <c r="D113" s="4"/>
@@ -3892,10 +3939,10 @@
       <c r="I113" s="4"/>
       <c r="J113" s="4"/>
     </row>
-    <row r="114" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A114" s="6"/>
-      <c r="B114" s="6"/>
-      <c r="C114" s="7" t="s">
+    <row r="114" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A114" s="11"/>
+      <c r="B114" s="11"/>
+      <c r="C114" s="6" t="s">
         <v>197</v>
       </c>
       <c r="D114" s="4"/>
@@ -3906,12 +3953,12 @@
       <c r="I114" s="4"/>
       <c r="J114" s="4"/>
     </row>
-    <row r="115" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A115" s="6"/>
-      <c r="B115" s="6" t="s">
+    <row r="115" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="11"/>
+      <c r="B115" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="C115" s="7" t="s">
+      <c r="C115" s="6" t="s">
         <v>200</v>
       </c>
       <c r="D115" s="4"/>
@@ -3922,10 +3969,10 @@
       <c r="I115" s="4"/>
       <c r="J115" s="4"/>
     </row>
-    <row r="116" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A116" s="6"/>
-      <c r="B116" s="6"/>
-      <c r="C116" s="7" t="s">
+    <row r="116" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="11"/>
+      <c r="B116" s="11"/>
+      <c r="C116" s="6" t="s">
         <v>201</v>
       </c>
       <c r="D116" s="4"/>
@@ -3936,10 +3983,10 @@
       <c r="I116" s="4"/>
       <c r="J116" s="4"/>
     </row>
-    <row r="117" spans="1:10" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A117" s="6"/>
-      <c r="B117" s="6"/>
-      <c r="C117" s="7" t="s">
+    <row r="117" spans="1:10" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A117" s="11"/>
+      <c r="B117" s="11"/>
+      <c r="C117" s="6" t="s">
         <v>202</v>
       </c>
       <c r="D117" s="4"/>
@@ -3950,10 +3997,10 @@
       <c r="I117" s="4"/>
       <c r="J117" s="4"/>
     </row>
-    <row r="118" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A118" s="6"/>
-      <c r="B118" s="6"/>
-      <c r="C118" s="7" t="s">
+    <row r="118" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A118" s="11"/>
+      <c r="B118" s="11"/>
+      <c r="C118" s="6" t="s">
         <v>203</v>
       </c>
       <c r="D118" s="4"/>
@@ -3964,10 +4011,10 @@
       <c r="I118" s="4"/>
       <c r="J118" s="4"/>
     </row>
-    <row r="119" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A119" s="6"/>
-      <c r="B119" s="6"/>
-      <c r="C119" s="7" t="s">
+    <row r="119" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A119" s="11"/>
+      <c r="B119" s="11"/>
+      <c r="C119" s="6" t="s">
         <v>204</v>
       </c>
       <c r="D119" s="4"/>
@@ -3978,10 +4025,10 @@
       <c r="I119" s="4"/>
       <c r="J119" s="4"/>
     </row>
-    <row r="120" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A120" s="6"/>
-      <c r="B120" s="6"/>
-      <c r="C120" s="7" t="s">
+    <row r="120" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A120" s="11"/>
+      <c r="B120" s="11"/>
+      <c r="C120" s="6" t="s">
         <v>205</v>
       </c>
       <c r="D120" s="4"/>
@@ -3992,10 +4039,10 @@
       <c r="I120" s="4"/>
       <c r="J120" s="4"/>
     </row>
-    <row r="121" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A121" s="6"/>
-      <c r="B121" s="6"/>
-      <c r="C121" s="7" t="s">
+    <row r="121" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A121" s="11"/>
+      <c r="B121" s="11"/>
+      <c r="C121" s="6" t="s">
         <v>206</v>
       </c>
       <c r="D121" s="4"/>
@@ -4006,10 +4053,10 @@
       <c r="I121" s="4"/>
       <c r="J121" s="4"/>
     </row>
-    <row r="122" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A122" s="6"/>
-      <c r="B122" s="6"/>
-      <c r="C122" s="7" t="s">
+    <row r="122" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A122" s="11"/>
+      <c r="B122" s="11"/>
+      <c r="C122" s="6" t="s">
         <v>207</v>
       </c>
       <c r="D122" s="4"/>
@@ -4020,10 +4067,10 @@
       <c r="I122" s="4"/>
       <c r="J122" s="4"/>
     </row>
-    <row r="123" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A123" s="6"/>
-      <c r="B123" s="6"/>
-      <c r="C123" s="7" t="s">
+    <row r="123" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A123" s="11"/>
+      <c r="B123" s="11"/>
+      <c r="C123" s="6" t="s">
         <v>208</v>
       </c>
       <c r="D123" s="4"/>
@@ -4034,10 +4081,10 @@
       <c r="I123" s="4"/>
       <c r="J123" s="4"/>
     </row>
-    <row r="124" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A124" s="6"/>
-      <c r="B124" s="6"/>
-      <c r="C124" s="7" t="s">
+    <row r="124" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A124" s="11"/>
+      <c r="B124" s="11"/>
+      <c r="C124" s="6" t="s">
         <v>209</v>
       </c>
       <c r="D124" s="4"/>
@@ -4048,10 +4095,10 @@
       <c r="I124" s="4"/>
       <c r="J124" s="4"/>
     </row>
-    <row r="125" spans="1:10" ht="18.399999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A125" s="6"/>
-      <c r="B125" s="6"/>
-      <c r="C125" s="7" t="s">
+    <row r="125" spans="1:10" ht="18.399999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A125" s="11"/>
+      <c r="B125" s="11"/>
+      <c r="C125" s="6" t="s">
         <v>210</v>
       </c>
       <c r="D125" s="4"/>
@@ -4062,10 +4109,10 @@
       <c r="I125" s="4"/>
       <c r="J125" s="4"/>
     </row>
-    <row r="126" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A126" s="6"/>
-      <c r="B126" s="6"/>
-      <c r="C126" s="7" t="s">
+    <row r="126" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A126" s="11"/>
+      <c r="B126" s="11"/>
+      <c r="C126" s="6" t="s">
         <v>211</v>
       </c>
       <c r="D126" s="4"/>
@@ -4076,10 +4123,10 @@
       <c r="I126" s="4"/>
       <c r="J126" s="4"/>
     </row>
-    <row r="127" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A127" s="6"/>
-      <c r="B127" s="6"/>
-      <c r="C127" s="7" t="s">
+    <row r="127" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A127" s="11"/>
+      <c r="B127" s="11"/>
+      <c r="C127" s="6" t="s">
         <v>212</v>
       </c>
       <c r="D127" s="4"/>
@@ -4090,10 +4137,10 @@
       <c r="I127" s="4"/>
       <c r="J127" s="4"/>
     </row>
-    <row r="128" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A128" s="6"/>
-      <c r="B128" s="6"/>
-      <c r="C128" s="7" t="s">
+    <row r="128" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A128" s="11"/>
+      <c r="B128" s="11"/>
+      <c r="C128" s="6" t="s">
         <v>213</v>
       </c>
       <c r="D128" s="4"/>
@@ -4104,10 +4151,10 @@
       <c r="I128" s="4"/>
       <c r="J128" s="4"/>
     </row>
-    <row r="129" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A129" s="6"/>
-      <c r="B129" s="6"/>
-      <c r="C129" s="7" t="s">
+    <row r="129" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A129" s="11"/>
+      <c r="B129" s="11"/>
+      <c r="C129" s="6" t="s">
         <v>214</v>
       </c>
       <c r="D129" s="4"/>
@@ -4118,10 +4165,10 @@
       <c r="I129" s="4"/>
       <c r="J129" s="4"/>
     </row>
-    <row r="130" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A130" s="6"/>
-      <c r="B130" s="6"/>
-      <c r="C130" s="7" t="s">
+    <row r="130" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A130" s="11"/>
+      <c r="B130" s="11"/>
+      <c r="C130" s="6" t="s">
         <v>216</v>
       </c>
       <c r="D130" s="4"/>
@@ -4132,10 +4179,10 @@
       <c r="I130" s="4"/>
       <c r="J130" s="4"/>
     </row>
-    <row r="131" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A131" s="6"/>
-      <c r="B131" s="6"/>
-      <c r="C131" s="7" t="s">
+    <row r="131" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A131" s="11"/>
+      <c r="B131" s="11"/>
+      <c r="C131" s="6" t="s">
         <v>217</v>
       </c>
       <c r="D131" s="4"/>
@@ -4146,10 +4193,10 @@
       <c r="I131" s="4"/>
       <c r="J131" s="4"/>
     </row>
-    <row r="132" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A132" s="6"/>
-      <c r="B132" s="6"/>
-      <c r="C132" s="7" t="s">
+    <row r="132" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A132" s="11"/>
+      <c r="B132" s="11"/>
+      <c r="C132" s="6" t="s">
         <v>218</v>
       </c>
       <c r="D132" s="4"/>
@@ -4160,10 +4207,10 @@
       <c r="I132" s="4"/>
       <c r="J132" s="4"/>
     </row>
-    <row r="133" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A133" s="6"/>
-      <c r="B133" s="6"/>
-      <c r="C133" s="7" t="s">
+    <row r="133" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A133" s="11"/>
+      <c r="B133" s="11"/>
+      <c r="C133" s="6" t="s">
         <v>215</v>
       </c>
       <c r="D133" s="4"/>
@@ -4174,14 +4221,14 @@
       <c r="I133" s="4"/>
       <c r="J133" s="4"/>
     </row>
-    <row r="134" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A134" s="6" t="s">
+    <row r="134" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A134" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B134" s="11" t="s">
+      <c r="B134" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="C134" s="7" t="s">
+      <c r="C134" s="6" t="s">
         <v>226</v>
       </c>
       <c r="D134" s="4"/>
@@ -4192,10 +4239,10 @@
       <c r="I134" s="4"/>
       <c r="J134" s="4"/>
     </row>
-    <row r="135" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A135" s="6"/>
-      <c r="B135" s="12"/>
-      <c r="C135" s="7"/>
+    <row r="135" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A135" s="11"/>
+      <c r="B135" s="13"/>
+      <c r="C135" s="6"/>
       <c r="D135" s="4"/>
       <c r="E135" s="4"/>
       <c r="F135" s="4"/>
@@ -4204,10 +4251,10 @@
       <c r="I135" s="4"/>
       <c r="J135" s="4"/>
     </row>
-    <row r="136" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A136" s="6"/>
-      <c r="B136" s="13"/>
-      <c r="C136" s="7"/>
+    <row r="136" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A136" s="11"/>
+      <c r="B136" s="14"/>
+      <c r="C136" s="6"/>
       <c r="D136" s="4"/>
       <c r="E136" s="4"/>
       <c r="F136" s="4"/>
@@ -4216,12 +4263,12 @@
       <c r="I136" s="4"/>
       <c r="J136" s="4"/>
     </row>
-    <row r="137" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A137" s="6"/>
-      <c r="B137" s="11" t="s">
+    <row r="137" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A137" s="11"/>
+      <c r="B137" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="C137" s="7"/>
+      <c r="C137" s="6"/>
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
       <c r="F137" s="4"/>
@@ -4230,10 +4277,10 @@
       <c r="I137" s="4"/>
       <c r="J137" s="4"/>
     </row>
-    <row r="138" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A138" s="6"/>
-      <c r="B138" s="12"/>
-      <c r="C138" s="7"/>
+    <row r="138" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A138" s="11"/>
+      <c r="B138" s="13"/>
+      <c r="C138" s="6"/>
       <c r="D138" s="4"/>
       <c r="E138" s="4"/>
       <c r="F138" s="4"/>
@@ -4242,10 +4289,10 @@
       <c r="I138" s="4"/>
       <c r="J138" s="4"/>
     </row>
-    <row r="139" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A139" s="6"/>
-      <c r="B139" s="13"/>
-      <c r="C139" s="7"/>
+    <row r="139" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A139" s="11"/>
+      <c r="B139" s="14"/>
+      <c r="C139" s="6"/>
       <c r="D139" s="4"/>
       <c r="E139" s="4"/>
       <c r="F139" s="4"/>
@@ -4254,12 +4301,12 @@
       <c r="I139" s="4"/>
       <c r="J139" s="4"/>
     </row>
-    <row r="140" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A140" s="6"/>
-      <c r="B140" s="11" t="s">
+    <row r="140" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A140" s="11"/>
+      <c r="B140" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="C140" s="7"/>
+      <c r="C140" s="6"/>
       <c r="D140" s="4"/>
       <c r="E140" s="4"/>
       <c r="F140" s="4"/>
@@ -4268,10 +4315,10 @@
       <c r="I140" s="4"/>
       <c r="J140" s="4"/>
     </row>
-    <row r="141" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A141" s="6"/>
-      <c r="B141" s="12"/>
-      <c r="C141" s="7"/>
+    <row r="141" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A141" s="11"/>
+      <c r="B141" s="13"/>
+      <c r="C141" s="6"/>
       <c r="D141" s="4"/>
       <c r="E141" s="4"/>
       <c r="F141" s="4"/>
@@ -4280,10 +4327,10 @@
       <c r="I141" s="4"/>
       <c r="J141" s="4"/>
     </row>
-    <row r="142" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A142" s="6"/>
-      <c r="B142" s="12"/>
-      <c r="C142" s="7"/>
+    <row r="142" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A142" s="11"/>
+      <c r="B142" s="13"/>
+      <c r="C142" s="6"/>
       <c r="D142" s="4"/>
       <c r="E142" s="4"/>
       <c r="F142" s="4"/>
@@ -4292,10 +4339,10 @@
       <c r="I142" s="4"/>
       <c r="J142" s="4"/>
     </row>
-    <row r="143" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A143" s="6"/>
-      <c r="B143" s="13"/>
-      <c r="C143" s="7"/>
+    <row r="143" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A143" s="11"/>
+      <c r="B143" s="14"/>
+      <c r="C143" s="6"/>
       <c r="D143" s="4"/>
       <c r="E143" s="4"/>
       <c r="F143" s="4"/>
@@ -4304,12 +4351,12 @@
       <c r="I143" s="4"/>
       <c r="J143" s="4"/>
     </row>
-    <row r="144" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A144" s="6"/>
-      <c r="B144" s="11" t="s">
+    <row r="144" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A144" s="11"/>
+      <c r="B144" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="C144" s="7"/>
+      <c r="C144" s="6"/>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
       <c r="F144" s="4"/>
@@ -4318,10 +4365,10 @@
       <c r="I144" s="4"/>
       <c r="J144" s="4"/>
     </row>
-    <row r="145" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A145" s="6"/>
-      <c r="B145" s="12"/>
-      <c r="C145" s="7"/>
+    <row r="145" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A145" s="11"/>
+      <c r="B145" s="13"/>
+      <c r="C145" s="6"/>
       <c r="D145" s="4"/>
       <c r="E145" s="4"/>
       <c r="F145" s="4"/>
@@ -4330,10 +4377,10 @@
       <c r="I145" s="4"/>
       <c r="J145" s="4"/>
     </row>
-    <row r="146" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A146" s="6"/>
-      <c r="B146" s="13"/>
-      <c r="C146" s="7"/>
+    <row r="146" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A146" s="11"/>
+      <c r="B146" s="14"/>
+      <c r="C146" s="6"/>
       <c r="D146" s="4"/>
       <c r="E146" s="4"/>
       <c r="F146" s="4"/>
@@ -4342,12 +4389,12 @@
       <c r="I146" s="4"/>
       <c r="J146" s="4"/>
     </row>
-    <row r="147" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A147" s="6"/>
-      <c r="B147" s="8" t="s">
+    <row r="147" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A147" s="11"/>
+      <c r="B147" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="C147" s="7"/>
+      <c r="C147" s="6"/>
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
       <c r="F147" s="4"/>
@@ -4356,12 +4403,12 @@
       <c r="I147" s="4"/>
       <c r="J147" s="4"/>
     </row>
-    <row r="148" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A148" s="6"/>
-      <c r="B148" s="11" t="s">
+    <row r="148" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A148" s="11"/>
+      <c r="B148" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="C148" s="7"/>
+      <c r="C148" s="6"/>
       <c r="D148" s="4"/>
       <c r="E148" s="4"/>
       <c r="F148" s="4"/>
@@ -4370,10 +4417,10 @@
       <c r="I148" s="4"/>
       <c r="J148" s="4"/>
     </row>
-    <row r="149" spans="1:10" ht="16.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A149" s="6"/>
-      <c r="B149" s="13"/>
-      <c r="C149" s="7"/>
+    <row r="149" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A149" s="11"/>
+      <c r="B149" s="14"/>
+      <c r="C149" s="6"/>
       <c r="D149" s="4"/>
       <c r="E149" s="4"/>
       <c r="F149" s="4"/>
@@ -4382,19 +4429,9 @@
       <c r="I149" s="4"/>
       <c r="J149" s="4"/>
     </row>
-    <row r="150" spans="1:10" ht="14.25" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="150" spans="1:10" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B115:B133"/>
-    <mergeCell ref="B134:B136"/>
-    <mergeCell ref="B137:B139"/>
-    <mergeCell ref="B140:B143"/>
-    <mergeCell ref="B144:B146"/>
-    <mergeCell ref="B148:B149"/>
-    <mergeCell ref="B70:B77"/>
-    <mergeCell ref="B78:B82"/>
-    <mergeCell ref="B83:B97"/>
-    <mergeCell ref="B98:B114"/>
     <mergeCell ref="A134:A149"/>
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="B10:B15"/>
@@ -4403,6 +4440,16 @@
     <mergeCell ref="B27:B58"/>
     <mergeCell ref="B59:B69"/>
     <mergeCell ref="A2:A133"/>
+    <mergeCell ref="B148:B149"/>
+    <mergeCell ref="B70:B77"/>
+    <mergeCell ref="B78:B82"/>
+    <mergeCell ref="B83:B97"/>
+    <mergeCell ref="B98:B114"/>
+    <mergeCell ref="B115:B133"/>
+    <mergeCell ref="B134:B136"/>
+    <mergeCell ref="B137:B139"/>
+    <mergeCell ref="B140:B143"/>
+    <mergeCell ref="B144:B146"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
annoate the finished task
</commit_message>
<xml_diff>
--- a/EDA_database_algorithm.xlsx
+++ b/EDA_database_algorithm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\respo\iEDA-standard-develop-codebase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA013882-5810-4325-96DD-7E5158110E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CA2471-F447-44A8-B2F1-AFC4E49FA9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{5A250FBF-FD77-48BD-871A-3834DD962A5A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{5A250FBF-FD77-48BD-871A-3834DD962A5A}"/>
   </bookViews>
   <sheets>
     <sheet name="数据结构" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="239">
   <si>
     <t>EDA数据结构</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -471,10 +471,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>最短路</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>第k条最短路</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -938,10 +934,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>李英奇</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>一般</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -950,6 +942,38 @@
   </si>
   <si>
     <t>见文档</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陈英奇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>常用字符串处理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串Hash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串tire字典树</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串Kmp算法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最短路(Floyd)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最短路(dijkstra)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1133,20 +1157,20 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1465,8 +1489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7543B24A-7FB2-4879-9E7B-EB413EED23FE}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1505,7 +1529,7 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -1528,148 +1552,196 @@
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="D3" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="I3" s="12">
+        <v>44472</v>
+      </c>
+      <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E4" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="I4" s="12">
+        <v>44473</v>
+      </c>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="E5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="G5" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="I5" s="12">
+        <v>44472</v>
+      </c>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="I4" s="16">
-        <v>44473</v>
-      </c>
-      <c r="J4" s="16"/>
-    </row>
-    <row r="5" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="F6" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="I6" s="12">
+        <v>44475</v>
+      </c>
+      <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="4" t="s">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="D7" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="I7" s="12">
+        <v>44475</v>
+      </c>
+      <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E8" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="I8" s="16">
+      <c r="I8" s="12">
         <v>44483</v>
       </c>
       <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E9" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="I9" s="16">
+      <c r="I9" s="12">
         <v>44492</v>
       </c>
       <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
@@ -1682,8 +1754,8 @@
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="4" t="s">
         <v>40</v>
       </c>
@@ -1696,8 +1768,8 @@
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="4" t="s">
         <v>41</v>
       </c>
@@ -1710,8 +1782,8 @@
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="4" t="s">
         <v>18</v>
       </c>
@@ -1724,8 +1796,8 @@
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12" t="s">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -1740,8 +1812,8 @@
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
@@ -1754,8 +1826,8 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="15.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="6" t="s">
         <v>23</v>
       </c>
@@ -1768,8 +1840,8 @@
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="6" t="s">
         <v>24</v>
       </c>
@@ -1782,8 +1854,8 @@
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="6" t="s">
         <v>25</v>
       </c>
@@ -1796,8 +1868,8 @@
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="6" t="s">
         <v>26</v>
       </c>
@@ -1810,8 +1882,8 @@
       <c r="J19" s="4"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="6" t="s">
         <v>31</v>
       </c>
@@ -1824,8 +1896,8 @@
       <c r="J20" s="4"/>
     </row>
     <row r="21" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="6" t="s">
         <v>27</v>
       </c>
@@ -1838,8 +1910,8 @@
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12" t="s">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13" t="s">
         <v>42</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -1854,8 +1926,8 @@
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="6" t="s">
         <v>33</v>
       </c>
@@ -1868,8 +1940,8 @@
       <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="6" t="s">
         <v>34</v>
       </c>
@@ -1882,8 +1954,8 @@
       <c r="J24" s="4"/>
     </row>
     <row r="25" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="6" t="s">
         <v>35</v>
       </c>
@@ -1896,8 +1968,8 @@
       <c r="J25" s="4"/>
     </row>
     <row r="26" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="6" t="s">
         <v>36</v>
       </c>
@@ -1910,8 +1982,8 @@
       <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="6" t="s">
         <v>37</v>
       </c>
@@ -1924,8 +1996,8 @@
       <c r="J27" s="4"/>
     </row>
     <row r="28" spans="1:10" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="6" t="s">
         <v>43</v>
       </c>
@@ -1938,8 +2010,8 @@
       <c r="J28" s="4"/>
     </row>
     <row r="29" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="6" t="s">
         <v>44</v>
       </c>
@@ -1952,8 +2024,8 @@
       <c r="J29" s="4"/>
     </row>
     <row r="30" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="6" t="s">
         <v>45</v>
       </c>
@@ -1966,8 +2038,8 @@
       <c r="J30" s="4"/>
     </row>
     <row r="31" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="6" t="s">
         <v>38</v>
       </c>
@@ -1980,10 +2052,10 @@
       <c r="J31" s="4"/>
     </row>
     <row r="32" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -1994,8 +2066,8 @@
       <c r="J32" s="4"/>
     </row>
     <row r="33" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
       <c r="C33" s="6" t="s">
         <v>67</v>
       </c>
@@ -2008,8 +2080,8 @@
       <c r="J33" s="4"/>
     </row>
     <row r="34" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12" t="s">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13" t="s">
         <v>47</v>
       </c>
       <c r="C34" s="6" t="s">
@@ -2024,8 +2096,8 @@
       <c r="J34" s="4"/>
     </row>
     <row r="35" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
       <c r="C35" s="6" t="s">
         <v>48</v>
       </c>
@@ -2038,8 +2110,8 @@
       <c r="J35" s="4"/>
     </row>
     <row r="36" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
       <c r="C36" s="6" t="s">
         <v>49</v>
       </c>
@@ -2052,8 +2124,8 @@
       <c r="J36" s="4"/>
     </row>
     <row r="37" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
       <c r="C37" s="6" t="s">
         <v>51</v>
       </c>
@@ -2066,8 +2138,8 @@
       <c r="J37" s="4"/>
     </row>
     <row r="38" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
       <c r="C38" s="6" t="s">
         <v>52</v>
       </c>
@@ -2080,7 +2152,7 @@
       <c r="J38" s="4"/>
     </row>
     <row r="39" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -2098,8 +2170,8 @@
       <c r="J39" s="4"/>
     </row>
     <row r="40" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12" t="s">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C40" s="6" t="s">
@@ -2114,8 +2186,8 @@
       <c r="J40" s="4"/>
     </row>
     <row r="41" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
       <c r="C41" s="6" t="s">
         <v>62</v>
       </c>
@@ -2128,8 +2200,8 @@
       <c r="J41" s="4"/>
     </row>
     <row r="42" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
       <c r="C42" s="6" t="s">
         <v>56</v>
       </c>
@@ -2142,8 +2214,8 @@
       <c r="J42" s="4"/>
     </row>
     <row r="43" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
       <c r="C43" s="6" t="s">
         <v>65</v>
       </c>
@@ -2156,8 +2228,8 @@
       <c r="J43" s="4"/>
     </row>
     <row r="44" spans="1:10" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
       <c r="C44" s="6" t="s">
         <v>66</v>
       </c>
@@ -2170,8 +2242,8 @@
       <c r="J44" s="4"/>
     </row>
     <row r="45" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
       <c r="C45" s="6" t="s">
         <v>63</v>
       </c>
@@ -2184,8 +2256,8 @@
       <c r="J45" s="4"/>
     </row>
     <row r="46" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12" t="s">
+      <c r="A46" s="13"/>
+      <c r="B46" s="13" t="s">
         <v>55</v>
       </c>
       <c r="C46" s="6" t="s">
@@ -2200,8 +2272,8 @@
       <c r="J46" s="4"/>
     </row>
     <row r="47" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
       <c r="C47" s="6" t="s">
         <v>59</v>
       </c>
@@ -2214,8 +2286,8 @@
       <c r="J47" s="4"/>
     </row>
     <row r="48" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
       <c r="C48" s="6" t="s">
         <v>60</v>
       </c>
@@ -2228,8 +2300,8 @@
       <c r="J48" s="4"/>
     </row>
     <row r="49" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
+      <c r="A49" s="13"/>
+      <c r="B49" s="13"/>
       <c r="C49" s="6" t="s">
         <v>61</v>
       </c>
@@ -2242,8 +2314,8 @@
       <c r="J49" s="4"/>
     </row>
     <row r="50" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12"/>
+      <c r="A50" s="13"/>
+      <c r="B50" s="13"/>
       <c r="C50" s="6" t="s">
         <v>64</v>
       </c>
@@ -2256,8 +2328,8 @@
       <c r="J50" s="4"/>
     </row>
     <row r="51" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="13"/>
       <c r="C51" s="6" t="s">
         <v>68</v>
       </c>
@@ -2290,10 +2362,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1B1B9C-0591-4BED-8FBD-040911B92B66}">
-  <dimension ref="A1:J150"/>
+  <dimension ref="A1:J155"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E136" sqref="E136"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2303,6 +2375,7 @@
     <col min="3" max="3" width="20.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.9140625" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="9.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2338,78 +2411,120 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="I2" s="12">
+        <v>44444</v>
+      </c>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="13"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="I3" s="12">
+        <v>44449</v>
+      </c>
+      <c r="J3" s="12"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="13"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="I4" s="12">
+        <v>44455</v>
+      </c>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="13"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="I5" s="12">
+        <v>44468</v>
+      </c>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
@@ -2422,10 +2537,10 @@
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
@@ -2438,16 +2553,14 @@
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>83</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -2456,14 +2569,14 @@
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -2471,59 +2584,65 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12" t="s">
-        <v>85</v>
-      </c>
+    <row r="10" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="4" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
+    <row r="11" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
+    <row r="12" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+        <v>81</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="6" t="s">
-        <v>89</v>
+    <row r="13" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -2532,10 +2651,12 @@
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13" t="s">
+        <v>85</v>
+      </c>
       <c r="C14" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -2546,10 +2667,10 @@
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="6" t="s">
-        <v>91</v>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -2560,19 +2681,13 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -2580,14 +2695,14 @@
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
-        <v>97</v>
+        <v>20</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -2596,15 +2711,13 @@
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="10" t="s">
-        <v>96</v>
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="D18" s="4"/>
-      <c r="E18" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -2612,15 +2725,13 @@
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="6" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="4" t="s">
-        <v>99</v>
-      </c>
+      <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
@@ -2628,14 +2739,18 @@
       <c r="J19" s="4"/>
     </row>
     <row r="20" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="C20" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20" s="4"/>
+        <v>102</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="E20" s="4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -2644,14 +2759,14 @@
       <c r="J20" s="4"/>
     </row>
     <row r="21" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="6" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -2660,15 +2775,15 @@
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>104</v>
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="10" t="s">
+        <v>96</v>
       </c>
       <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -2676,13 +2791,15 @@
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="6" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -2690,13 +2807,15 @@
       <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="6" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+      <c r="E24" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -2704,13 +2823,15 @@
       <c r="J24" s="4"/>
     </row>
     <row r="25" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -2718,10 +2839,12 @@
       <c r="J25" s="4"/>
     </row>
     <row r="26" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="13" t="s">
+        <v>20</v>
+      </c>
       <c r="C26" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -2732,12 +2855,10 @@
       <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12" t="s">
-        <v>42</v>
-      </c>
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -2748,10 +2869,10 @@
       <c r="J27" s="4"/>
     </row>
     <row r="28" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -2762,10 +2883,10 @@
       <c r="J28" s="4"/>
     </row>
     <row r="29" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -2776,10 +2897,10 @@
       <c r="J29" s="4"/>
     </row>
     <row r="30" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -2790,10 +2911,12 @@
       <c r="J30" s="4"/>
     </row>
     <row r="31" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="C31" s="6" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -2804,10 +2927,10 @@
       <c r="J31" s="4"/>
     </row>
     <row r="32" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -2818,10 +2941,10 @@
       <c r="J32" s="4"/>
     </row>
     <row r="33" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
       <c r="C33" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -2832,38 +2955,62 @@
       <c r="J33" s="4"/>
     </row>
     <row r="34" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="I34" s="12">
+        <v>44471</v>
+      </c>
+      <c r="J34" s="12"/>
     </row>
     <row r="35" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="I35" s="12">
+        <v>44471</v>
+      </c>
+      <c r="J35" s="12"/>
     </row>
     <row r="36" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
       <c r="C36" s="6" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -2874,10 +3021,10 @@
       <c r="J36" s="4"/>
     </row>
     <row r="37" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
       <c r="C37" s="6" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -2888,10 +3035,10 @@
       <c r="J37" s="4"/>
     </row>
     <row r="38" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
       <c r="C38" s="6" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -2902,10 +3049,10 @@
       <c r="J38" s="4"/>
     </row>
     <row r="39" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
       <c r="C39" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -2916,10 +3063,10 @@
       <c r="J39" s="4"/>
     </row>
     <row r="40" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
       <c r="C40" s="6" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -2930,8 +3077,8 @@
       <c r="J40" s="4"/>
     </row>
     <row r="41" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
       <c r="C41" s="6" t="s">
         <v>121</v>
       </c>
@@ -2944,10 +3091,10 @@
       <c r="J41" s="4"/>
     </row>
     <row r="42" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
       <c r="C42" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -2958,10 +3105,10 @@
       <c r="J42" s="4"/>
     </row>
     <row r="43" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
       <c r="C43" s="6" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -2972,10 +3119,10 @@
       <c r="J43" s="4"/>
     </row>
     <row r="44" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
       <c r="C44" s="6" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -2986,10 +3133,10 @@
       <c r="J44" s="4"/>
     </row>
     <row r="45" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
       <c r="C45" s="6" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -3000,10 +3147,10 @@
       <c r="J45" s="4"/>
     </row>
     <row r="46" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
       <c r="C46" s="6" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -3014,10 +3161,10 @@
       <c r="J46" s="4"/>
     </row>
     <row r="47" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
       <c r="C47" s="6" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
@@ -3028,10 +3175,10 @@
       <c r="J47" s="4"/>
     </row>
     <row r="48" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
       <c r="C48" s="6" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -3042,10 +3189,10 @@
       <c r="J48" s="4"/>
     </row>
     <row r="49" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
+      <c r="A49" s="13"/>
+      <c r="B49" s="13"/>
       <c r="C49" s="6" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -3056,10 +3203,10 @@
       <c r="J49" s="4"/>
     </row>
     <row r="50" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12"/>
+      <c r="A50" s="13"/>
+      <c r="B50" s="13"/>
       <c r="C50" s="6" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -3070,10 +3217,10 @@
       <c r="J50" s="4"/>
     </row>
     <row r="51" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="13"/>
       <c r="C51" s="6" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -3084,10 +3231,10 @@
       <c r="J51" s="4"/>
     </row>
     <row r="52" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
+      <c r="A52" s="13"/>
+      <c r="B52" s="13"/>
       <c r="C52" s="6" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -3098,10 +3245,10 @@
       <c r="J52" s="4"/>
     </row>
     <row r="53" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12"/>
+      <c r="A53" s="13"/>
+      <c r="B53" s="13"/>
       <c r="C53" s="6" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -3112,10 +3259,10 @@
       <c r="J53" s="4"/>
     </row>
     <row r="54" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12"/>
+      <c r="A54" s="13"/>
+      <c r="B54" s="13"/>
       <c r="C54" s="6" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -3126,10 +3273,10 @@
       <c r="J54" s="4"/>
     </row>
     <row r="55" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12"/>
+      <c r="A55" s="13"/>
+      <c r="B55" s="13"/>
       <c r="C55" s="6" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -3140,10 +3287,10 @@
       <c r="J55" s="4"/>
     </row>
     <row r="56" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="12"/>
-      <c r="B56" s="12"/>
+      <c r="A56" s="13"/>
+      <c r="B56" s="13"/>
       <c r="C56" s="6" t="s">
-        <v>178</v>
+        <v>132</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
@@ -3154,10 +3301,10 @@
       <c r="J56" s="4"/>
     </row>
     <row r="57" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="12"/>
-      <c r="B57" s="12"/>
+      <c r="A57" s="13"/>
+      <c r="B57" s="13"/>
       <c r="C57" s="6" t="s">
-        <v>177</v>
+        <v>133</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
@@ -3168,8 +3315,8 @@
       <c r="J57" s="4"/>
     </row>
     <row r="58" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="12"/>
-      <c r="B58" s="12"/>
+      <c r="A58" s="13"/>
+      <c r="B58" s="13"/>
       <c r="C58" s="6" t="s">
         <v>135</v>
       </c>
@@ -3182,17 +3329,13 @@
       <c r="J58" s="4"/>
     </row>
     <row r="59" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="12"/>
-      <c r="B59" s="12" t="s">
-        <v>199</v>
-      </c>
+      <c r="A59" s="13"/>
+      <c r="B59" s="13"/>
       <c r="C59" s="6" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
       <c r="D59" s="4"/>
-      <c r="E59" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="E59" s="4"/>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
@@ -3200,15 +3343,13 @@
       <c r="J59" s="4"/>
     </row>
     <row r="60" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="12"/>
-      <c r="B60" s="12"/>
+      <c r="A60" s="13"/>
+      <c r="B60" s="13"/>
       <c r="C60" s="6" t="s">
-        <v>95</v>
+        <v>137</v>
       </c>
       <c r="D60" s="4"/>
-      <c r="E60" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="E60" s="4"/>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
@@ -3216,10 +3357,10 @@
       <c r="J60" s="4"/>
     </row>
     <row r="61" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="12"/>
-      <c r="B61" s="12"/>
+      <c r="A61" s="13"/>
+      <c r="B61" s="13"/>
       <c r="C61" s="6" t="s">
-        <v>140</v>
+        <v>177</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -3230,10 +3371,10 @@
       <c r="J61" s="4"/>
     </row>
     <row r="62" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="12"/>
-      <c r="B62" s="12"/>
+      <c r="A62" s="13"/>
+      <c r="B62" s="13"/>
       <c r="C62" s="6" t="s">
-        <v>141</v>
+        <v>176</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
@@ -3244,10 +3385,10 @@
       <c r="J62" s="4"/>
     </row>
     <row r="63" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="12"/>
-      <c r="B63" s="12"/>
+      <c r="A63" s="13"/>
+      <c r="B63" s="13"/>
       <c r="C63" s="6" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
@@ -3258,13 +3399,17 @@
       <c r="J63" s="4"/>
     </row>
     <row r="64" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="12"/>
-      <c r="B64" s="12"/>
+      <c r="A64" s="13"/>
+      <c r="B64" s="13" t="s">
+        <v>198</v>
+      </c>
       <c r="C64" s="6" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
       <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
+      <c r="E64" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
@@ -3272,13 +3417,15 @@
       <c r="J64" s="4"/>
     </row>
     <row r="65" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="12"/>
-      <c r="B65" s="12"/>
+      <c r="A65" s="13"/>
+      <c r="B65" s="13"/>
       <c r="C65" s="6" t="s">
-        <v>144</v>
+        <v>95</v>
       </c>
       <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
+      <c r="E65" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
@@ -3286,10 +3433,10 @@
       <c r="J65" s="4"/>
     </row>
     <row r="66" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="12"/>
-      <c r="B66" s="12"/>
+      <c r="A66" s="13"/>
+      <c r="B66" s="13"/>
       <c r="C66" s="6" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
@@ -3300,10 +3447,10 @@
       <c r="J66" s="4"/>
     </row>
     <row r="67" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="12"/>
-      <c r="B67" s="12"/>
+      <c r="A67" s="13"/>
+      <c r="B67" s="13"/>
       <c r="C67" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
@@ -3314,10 +3461,10 @@
       <c r="J67" s="4"/>
     </row>
     <row r="68" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="12"/>
-      <c r="B68" s="12"/>
+      <c r="A68" s="13"/>
+      <c r="B68" s="13"/>
       <c r="C68" s="6" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
@@ -3328,10 +3475,10 @@
       <c r="J68" s="4"/>
     </row>
     <row r="69" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="12"/>
-      <c r="B69" s="12"/>
+      <c r="A69" s="13"/>
+      <c r="B69" s="13"/>
       <c r="C69" s="6" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
@@ -3342,12 +3489,10 @@
       <c r="J69" s="4"/>
     </row>
     <row r="70" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="12"/>
-      <c r="B70" s="12" t="s">
-        <v>152</v>
-      </c>
+      <c r="A70" s="13"/>
+      <c r="B70" s="13"/>
       <c r="C70" s="6" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
@@ -3358,10 +3503,10 @@
       <c r="J70" s="4"/>
     </row>
     <row r="71" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="12"/>
-      <c r="B71" s="12"/>
+      <c r="A71" s="13"/>
+      <c r="B71" s="13"/>
       <c r="C71" s="6" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
@@ -3372,10 +3517,10 @@
       <c r="J71" s="4"/>
     </row>
     <row r="72" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="12"/>
-      <c r="B72" s="12"/>
+      <c r="A72" s="13"/>
+      <c r="B72" s="13"/>
       <c r="C72" s="6" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
@@ -3386,10 +3531,10 @@
       <c r="J72" s="4"/>
     </row>
     <row r="73" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="12"/>
-      <c r="B73" s="12"/>
+      <c r="A73" s="13"/>
+      <c r="B73" s="13"/>
       <c r="C73" s="6" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
@@ -3400,10 +3545,10 @@
       <c r="J73" s="4"/>
     </row>
     <row r="74" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="12"/>
-      <c r="B74" s="12"/>
+      <c r="A74" s="13"/>
+      <c r="B74" s="13"/>
       <c r="C74" s="6" t="s">
-        <v>181</v>
+        <v>149</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -3414,10 +3559,12 @@
       <c r="J74" s="4"/>
     </row>
     <row r="75" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="12"/>
-      <c r="B75" s="12"/>
+      <c r="A75" s="13"/>
+      <c r="B75" s="13" t="s">
+        <v>151</v>
+      </c>
       <c r="C75" s="6" t="s">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
@@ -3428,10 +3575,10 @@
       <c r="J75" s="4"/>
     </row>
     <row r="76" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="12"/>
-      <c r="B76" s="12"/>
+      <c r="A76" s="13"/>
+      <c r="B76" s="13"/>
       <c r="C76" s="6" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -3442,10 +3589,10 @@
       <c r="J76" s="4"/>
     </row>
     <row r="77" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="12"/>
-      <c r="B77" s="12"/>
+      <c r="A77" s="13"/>
+      <c r="B77" s="13"/>
       <c r="C77" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
@@ -3456,12 +3603,10 @@
       <c r="J77" s="4"/>
     </row>
     <row r="78" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="12"/>
-      <c r="B78" s="12" t="s">
-        <v>157</v>
-      </c>
+      <c r="A78" s="13"/>
+      <c r="B78" s="13"/>
       <c r="C78" s="6" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
@@ -3472,10 +3617,10 @@
       <c r="J78" s="4"/>
     </row>
     <row r="79" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="12"/>
-      <c r="B79" s="12"/>
+      <c r="A79" s="13"/>
+      <c r="B79" s="13"/>
       <c r="C79" s="6" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
@@ -3486,10 +3631,10 @@
       <c r="J79" s="4"/>
     </row>
     <row r="80" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="12"/>
-      <c r="B80" s="12"/>
+      <c r="A80" s="13"/>
+      <c r="B80" s="13"/>
       <c r="C80" s="6" t="s">
-        <v>160</v>
+        <v>179</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
@@ -3500,10 +3645,10 @@
       <c r="J80" s="4"/>
     </row>
     <row r="81" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="12"/>
-      <c r="B81" s="12"/>
+      <c r="A81" s="13"/>
+      <c r="B81" s="13"/>
       <c r="C81" s="6" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
@@ -3514,10 +3659,10 @@
       <c r="J81" s="4"/>
     </row>
     <row r="82" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="12"/>
-      <c r="B82" s="12"/>
+      <c r="A82" s="13"/>
+      <c r="B82" s="13"/>
       <c r="C82" s="6" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
@@ -3528,12 +3673,12 @@
       <c r="J82" s="4"/>
     </row>
     <row r="83" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="12"/>
-      <c r="B83" s="12" t="s">
-        <v>179</v>
+      <c r="A83" s="13"/>
+      <c r="B83" s="13" t="s">
+        <v>156</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="4"/>
@@ -3544,10 +3689,10 @@
       <c r="J83" s="4"/>
     </row>
     <row r="84" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="12"/>
-      <c r="B84" s="12"/>
+      <c r="A84" s="13"/>
+      <c r="B84" s="13"/>
       <c r="C84" s="6" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
@@ -3558,10 +3703,10 @@
       <c r="J84" s="4"/>
     </row>
     <row r="85" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="12"/>
-      <c r="B85" s="12"/>
+      <c r="A85" s="13"/>
+      <c r="B85" s="13"/>
       <c r="C85" s="6" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
@@ -3572,10 +3717,10 @@
       <c r="J85" s="4"/>
     </row>
     <row r="86" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="12"/>
-      <c r="B86" s="12"/>
+      <c r="A86" s="13"/>
+      <c r="B86" s="13"/>
       <c r="C86" s="6" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
@@ -3586,10 +3731,10 @@
       <c r="J86" s="4"/>
     </row>
     <row r="87" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="12"/>
-      <c r="B87" s="12"/>
+      <c r="A87" s="13"/>
+      <c r="B87" s="13"/>
       <c r="C87" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -3600,10 +3745,12 @@
       <c r="J87" s="4"/>
     </row>
     <row r="88" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="12"/>
-      <c r="B88" s="12"/>
+      <c r="A88" s="13"/>
+      <c r="B88" s="13" t="s">
+        <v>178</v>
+      </c>
       <c r="C88" s="6" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
@@ -3614,10 +3761,10 @@
       <c r="J88" s="4"/>
     </row>
     <row r="89" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="12"/>
-      <c r="B89" s="12"/>
+      <c r="A89" s="13"/>
+      <c r="B89" s="13"/>
       <c r="C89" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
@@ -3628,10 +3775,10 @@
       <c r="J89" s="4"/>
     </row>
     <row r="90" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="12"/>
-      <c r="B90" s="12"/>
+      <c r="A90" s="13"/>
+      <c r="B90" s="13"/>
       <c r="C90" s="6" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
@@ -3642,10 +3789,10 @@
       <c r="J90" s="4"/>
     </row>
     <row r="91" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="12"/>
-      <c r="B91" s="12"/>
+      <c r="A91" s="13"/>
+      <c r="B91" s="13"/>
       <c r="C91" s="6" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
@@ -3656,10 +3803,10 @@
       <c r="J91" s="4"/>
     </row>
     <row r="92" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="12"/>
-      <c r="B92" s="12"/>
+      <c r="A92" s="13"/>
+      <c r="B92" s="13"/>
       <c r="C92" s="6" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
@@ -3669,11 +3816,11 @@
       <c r="I92" s="4"/>
       <c r="J92" s="4"/>
     </row>
-    <row r="93" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="12"/>
-      <c r="B93" s="12"/>
+    <row r="93" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="13"/>
+      <c r="B93" s="13"/>
       <c r="C93" s="6" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
@@ -3683,11 +3830,11 @@
       <c r="I93" s="4"/>
       <c r="J93" s="4"/>
     </row>
-    <row r="94" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="12"/>
-      <c r="B94" s="12"/>
+    <row r="94" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="13"/>
+      <c r="B94" s="13"/>
       <c r="C94" s="6" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
@@ -3698,10 +3845,10 @@
       <c r="J94" s="4"/>
     </row>
     <row r="95" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="12"/>
-      <c r="B95" s="12"/>
+      <c r="A95" s="13"/>
+      <c r="B95" s="13"/>
       <c r="C95" s="6" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4"/>
@@ -3711,11 +3858,11 @@
       <c r="I95" s="4"/>
       <c r="J95" s="4"/>
     </row>
-    <row r="96" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="12"/>
-      <c r="B96" s="12"/>
+    <row r="96" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="13"/>
+      <c r="B96" s="13"/>
       <c r="C96" s="6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
@@ -3725,11 +3872,11 @@
       <c r="I96" s="4"/>
       <c r="J96" s="4"/>
     </row>
-    <row r="97" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="12"/>
-      <c r="B97" s="12"/>
+    <row r="97" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="13"/>
+      <c r="B97" s="13"/>
       <c r="C97" s="6" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
@@ -3739,13 +3886,11 @@
       <c r="I97" s="4"/>
       <c r="J97" s="4"/>
     </row>
-    <row r="98" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="12"/>
-      <c r="B98" s="12" t="s">
-        <v>198</v>
-      </c>
+    <row r="98" spans="1:10" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="13"/>
+      <c r="B98" s="13"/>
       <c r="C98" s="6" t="s">
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
@@ -3756,10 +3901,10 @@
       <c r="J98" s="4"/>
     </row>
     <row r="99" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="12"/>
-      <c r="B99" s="12"/>
+      <c r="A99" s="13"/>
+      <c r="B99" s="13"/>
       <c r="C99" s="6" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
@@ -3770,10 +3915,10 @@
       <c r="J99" s="4"/>
     </row>
     <row r="100" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="12"/>
-      <c r="B100" s="12"/>
+      <c r="A100" s="13"/>
+      <c r="B100" s="13"/>
       <c r="C100" s="6" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
@@ -3783,11 +3928,11 @@
       <c r="I100" s="4"/>
       <c r="J100" s="4"/>
     </row>
-    <row r="101" spans="1:10" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="12"/>
-      <c r="B101" s="12"/>
+    <row r="101" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="13"/>
+      <c r="B101" s="13"/>
       <c r="C101" s="6" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>
@@ -3798,10 +3943,10 @@
       <c r="J101" s="4"/>
     </row>
     <row r="102" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="12"/>
-      <c r="B102" s="12"/>
+      <c r="A102" s="13"/>
+      <c r="B102" s="13"/>
       <c r="C102" s="6" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="4"/>
@@ -3812,10 +3957,12 @@
       <c r="J102" s="4"/>
     </row>
     <row r="103" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="12"/>
-      <c r="B103" s="12"/>
+      <c r="A103" s="13"/>
+      <c r="B103" s="13" t="s">
+        <v>197</v>
+      </c>
       <c r="C103" s="6" t="s">
-        <v>186</v>
+        <v>90</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="4"/>
@@ -3826,10 +3973,10 @@
       <c r="J103" s="4"/>
     </row>
     <row r="104" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="12"/>
-      <c r="B104" s="12"/>
+      <c r="A104" s="13"/>
+      <c r="B104" s="13"/>
       <c r="C104" s="6" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D104" s="4"/>
       <c r="E104" s="4"/>
@@ -3840,10 +3987,10 @@
       <c r="J104" s="4"/>
     </row>
     <row r="105" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="12"/>
-      <c r="B105" s="12"/>
+      <c r="A105" s="13"/>
+      <c r="B105" s="13"/>
       <c r="C105" s="6" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D105" s="4"/>
       <c r="E105" s="4"/>
@@ -3853,11 +4000,11 @@
       <c r="I105" s="4"/>
       <c r="J105" s="4"/>
     </row>
-    <row r="106" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="12"/>
-      <c r="B106" s="12"/>
+    <row r="106" spans="1:10" ht="18.399999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A106" s="13"/>
+      <c r="B106" s="13"/>
       <c r="C106" s="6" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D106" s="4"/>
       <c r="E106" s="4"/>
@@ -3868,10 +4015,10 @@
       <c r="J106" s="4"/>
     </row>
     <row r="107" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="12"/>
-      <c r="B107" s="12"/>
+      <c r="A107" s="13"/>
+      <c r="B107" s="13"/>
       <c r="C107" s="6" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
@@ -3882,10 +4029,10 @@
       <c r="J107" s="4"/>
     </row>
     <row r="108" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="12"/>
-      <c r="B108" s="12"/>
+      <c r="A108" s="13"/>
+      <c r="B108" s="13"/>
       <c r="C108" s="6" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D108" s="4"/>
       <c r="E108" s="4"/>
@@ -3895,11 +4042,11 @@
       <c r="I108" s="4"/>
       <c r="J108" s="4"/>
     </row>
-    <row r="109" spans="1:10" ht="18.399999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="12"/>
-      <c r="B109" s="12"/>
+    <row r="109" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="13"/>
+      <c r="B109" s="13"/>
       <c r="C109" s="6" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
@@ -3910,10 +4057,10 @@
       <c r="J109" s="4"/>
     </row>
     <row r="110" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="12"/>
-      <c r="B110" s="12"/>
+      <c r="A110" s="13"/>
+      <c r="B110" s="13"/>
       <c r="C110" s="6" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
@@ -3924,10 +4071,10 @@
       <c r="J110" s="4"/>
     </row>
     <row r="111" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="12"/>
-      <c r="B111" s="12"/>
+      <c r="A111" s="13"/>
+      <c r="B111" s="13"/>
       <c r="C111" s="6" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
@@ -3938,10 +4085,10 @@
       <c r="J111" s="4"/>
     </row>
     <row r="112" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="12"/>
-      <c r="B112" s="12"/>
+      <c r="A112" s="13"/>
+      <c r="B112" s="13"/>
       <c r="C112" s="6" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
@@ -3952,10 +4099,10 @@
       <c r="J112" s="4"/>
     </row>
     <row r="113" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="12"/>
-      <c r="B113" s="12"/>
+      <c r="A113" s="13"/>
+      <c r="B113" s="13"/>
       <c r="C113" s="6" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
@@ -3965,11 +4112,11 @@
       <c r="I113" s="4"/>
       <c r="J113" s="4"/>
     </row>
-    <row r="114" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="12"/>
-      <c r="B114" s="12"/>
+    <row r="114" spans="1:10" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A114" s="13"/>
+      <c r="B114" s="13"/>
       <c r="C114" s="6" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D114" s="4"/>
       <c r="E114" s="4"/>
@@ -3980,12 +4127,10 @@
       <c r="J114" s="4"/>
     </row>
     <row r="115" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="12"/>
-      <c r="B115" s="12" t="s">
-        <v>219</v>
-      </c>
+      <c r="A115" s="13"/>
+      <c r="B115" s="13"/>
       <c r="C115" s="6" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
@@ -3996,10 +4141,10 @@
       <c r="J115" s="4"/>
     </row>
     <row r="116" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="12"/>
-      <c r="B116" s="12"/>
+      <c r="A116" s="13"/>
+      <c r="B116" s="13"/>
       <c r="C116" s="6" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
@@ -4009,11 +4154,11 @@
       <c r="I116" s="4"/>
       <c r="J116" s="4"/>
     </row>
-    <row r="117" spans="1:10" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="12"/>
-      <c r="B117" s="12"/>
+    <row r="117" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A117" s="13"/>
+      <c r="B117" s="13"/>
       <c r="C117" s="6" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
@@ -4024,10 +4169,10 @@
       <c r="J117" s="4"/>
     </row>
     <row r="118" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="12"/>
-      <c r="B118" s="12"/>
+      <c r="A118" s="13"/>
+      <c r="B118" s="13"/>
       <c r="C118" s="6" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
@@ -4038,10 +4183,10 @@
       <c r="J118" s="4"/>
     </row>
     <row r="119" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="12"/>
-      <c r="B119" s="12"/>
+      <c r="A119" s="13"/>
+      <c r="B119" s="13"/>
       <c r="C119" s="6" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
@@ -4052,10 +4197,12 @@
       <c r="J119" s="4"/>
     </row>
     <row r="120" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="12"/>
-      <c r="B120" s="12"/>
+      <c r="A120" s="13"/>
+      <c r="B120" s="13" t="s">
+        <v>218</v>
+      </c>
       <c r="C120" s="6" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D120" s="4"/>
       <c r="E120" s="4"/>
@@ -4066,10 +4213,10 @@
       <c r="J120" s="4"/>
     </row>
     <row r="121" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="12"/>
-      <c r="B121" s="12"/>
+      <c r="A121" s="13"/>
+      <c r="B121" s="13"/>
       <c r="C121" s="6" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
@@ -4079,11 +4226,11 @@
       <c r="I121" s="4"/>
       <c r="J121" s="4"/>
     </row>
-    <row r="122" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="12"/>
-      <c r="B122" s="12"/>
+    <row r="122" spans="1:10" ht="18.399999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A122" s="13"/>
+      <c r="B122" s="13"/>
       <c r="C122" s="6" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D122" s="4"/>
       <c r="E122" s="4"/>
@@ -4094,10 +4241,10 @@
       <c r="J122" s="4"/>
     </row>
     <row r="123" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="12"/>
-      <c r="B123" s="12"/>
+      <c r="A123" s="13"/>
+      <c r="B123" s="13"/>
       <c r="C123" s="6" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D123" s="4"/>
       <c r="E123" s="4"/>
@@ -4108,10 +4255,10 @@
       <c r="J123" s="4"/>
     </row>
     <row r="124" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="12"/>
-      <c r="B124" s="12"/>
+      <c r="A124" s="13"/>
+      <c r="B124" s="13"/>
       <c r="C124" s="6" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="D124" s="4"/>
       <c r="E124" s="4"/>
@@ -4121,11 +4268,11 @@
       <c r="I124" s="4"/>
       <c r="J124" s="4"/>
     </row>
-    <row r="125" spans="1:10" ht="18.399999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="12"/>
-      <c r="B125" s="12"/>
+    <row r="125" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A125" s="13"/>
+      <c r="B125" s="13"/>
       <c r="C125" s="6" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="4"/>
@@ -4136,10 +4283,10 @@
       <c r="J125" s="4"/>
     </row>
     <row r="126" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="12"/>
-      <c r="B126" s="12"/>
+      <c r="A126" s="13"/>
+      <c r="B126" s="13"/>
       <c r="C126" s="6" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D126" s="4"/>
       <c r="E126" s="4"/>
@@ -4150,10 +4297,10 @@
       <c r="J126" s="4"/>
     </row>
     <row r="127" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A127" s="12"/>
-      <c r="B127" s="12"/>
+      <c r="A127" s="13"/>
+      <c r="B127" s="13"/>
       <c r="C127" s="6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D127" s="4"/>
       <c r="E127" s="4"/>
@@ -4164,10 +4311,10 @@
       <c r="J127" s="4"/>
     </row>
     <row r="128" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="12"/>
-      <c r="B128" s="12"/>
+      <c r="A128" s="13"/>
+      <c r="B128" s="13"/>
       <c r="C128" s="6" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D128" s="4"/>
       <c r="E128" s="4"/>
@@ -4178,10 +4325,10 @@
       <c r="J128" s="4"/>
     </row>
     <row r="129" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="12"/>
-      <c r="B129" s="12"/>
+      <c r="A129" s="13"/>
+      <c r="B129" s="13"/>
       <c r="C129" s="6" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D129" s="4"/>
       <c r="E129" s="4"/>
@@ -4192,10 +4339,10 @@
       <c r="J129" s="4"/>
     </row>
     <row r="130" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="12"/>
-      <c r="B130" s="12"/>
+      <c r="A130" s="13"/>
+      <c r="B130" s="13"/>
       <c r="C130" s="6" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D130" s="4"/>
       <c r="E130" s="4"/>
@@ -4206,10 +4353,12 @@
       <c r="J130" s="4"/>
     </row>
     <row r="131" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="12"/>
-      <c r="B131" s="12"/>
+      <c r="A131" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B131" s="13"/>
       <c r="C131" s="6" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="D131" s="4"/>
       <c r="E131" s="4"/>
@@ -4220,10 +4369,10 @@
       <c r="J131" s="4"/>
     </row>
     <row r="132" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A132" s="12"/>
-      <c r="B132" s="12"/>
+      <c r="A132" s="13"/>
+      <c r="B132" s="13"/>
       <c r="C132" s="6" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D132" s="4"/>
       <c r="E132" s="4"/>
@@ -4234,10 +4383,10 @@
       <c r="J132" s="4"/>
     </row>
     <row r="133" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A133" s="12"/>
-      <c r="B133" s="12"/>
+      <c r="A133" s="13"/>
+      <c r="B133" s="13"/>
       <c r="C133" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="4"/>
@@ -4248,14 +4397,10 @@
       <c r="J133" s="4"/>
     </row>
     <row r="134" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B134" s="13" t="s">
-        <v>225</v>
-      </c>
+      <c r="A134" s="13"/>
+      <c r="B134" s="13"/>
       <c r="C134" s="6" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D134" s="4"/>
       <c r="E134" s="4"/>
@@ -4266,9 +4411,11 @@
       <c r="J134" s="4"/>
     </row>
     <row r="135" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="12"/>
-      <c r="B135" s="15"/>
-      <c r="C135" s="6"/>
+      <c r="A135" s="13"/>
+      <c r="B135" s="13"/>
+      <c r="C135" s="6" t="s">
+        <v>215</v>
+      </c>
       <c r="D135" s="4"/>
       <c r="E135" s="4"/>
       <c r="F135" s="4"/>
@@ -4278,9 +4425,11 @@
       <c r="J135" s="4"/>
     </row>
     <row r="136" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="12"/>
-      <c r="B136" s="14"/>
-      <c r="C136" s="6"/>
+      <c r="A136" s="13"/>
+      <c r="B136" s="13"/>
+      <c r="C136" s="6" t="s">
+        <v>216</v>
+      </c>
       <c r="D136" s="4"/>
       <c r="E136" s="4"/>
       <c r="F136" s="4"/>
@@ -4290,11 +4439,11 @@
       <c r="J136" s="4"/>
     </row>
     <row r="137" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="12"/>
-      <c r="B137" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="C137" s="6"/>
+      <c r="A137" s="13"/>
+      <c r="B137" s="13"/>
+      <c r="C137" s="6" t="s">
+        <v>217</v>
+      </c>
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
       <c r="F137" s="4"/>
@@ -4304,9 +4453,11 @@
       <c r="J137" s="4"/>
     </row>
     <row r="138" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="12"/>
-      <c r="B138" s="15"/>
-      <c r="C138" s="6"/>
+      <c r="A138" s="13"/>
+      <c r="B138" s="13"/>
+      <c r="C138" s="6" t="s">
+        <v>214</v>
+      </c>
       <c r="D138" s="4"/>
       <c r="E138" s="4"/>
       <c r="F138" s="4"/>
@@ -4316,9 +4467,13 @@
       <c r="J138" s="4"/>
     </row>
     <row r="139" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="12"/>
-      <c r="B139" s="14"/>
-      <c r="C139" s="6"/>
+      <c r="A139" s="13"/>
+      <c r="B139" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="C139" s="6" t="s">
+        <v>225</v>
+      </c>
       <c r="D139" s="4"/>
       <c r="E139" s="4"/>
       <c r="F139" s="4"/>
@@ -4328,10 +4483,8 @@
       <c r="J139" s="4"/>
     </row>
     <row r="140" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="12"/>
-      <c r="B140" s="13" t="s">
-        <v>221</v>
-      </c>
+      <c r="A140" s="13"/>
+      <c r="B140" s="15"/>
       <c r="C140" s="6"/>
       <c r="D140" s="4"/>
       <c r="E140" s="4"/>
@@ -4342,8 +4495,8 @@
       <c r="J140" s="4"/>
     </row>
     <row r="141" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="12"/>
-      <c r="B141" s="15"/>
+      <c r="A141" s="13"/>
+      <c r="B141" s="16"/>
       <c r="C141" s="6"/>
       <c r="D141" s="4"/>
       <c r="E141" s="4"/>
@@ -4354,8 +4507,10 @@
       <c r="J141" s="4"/>
     </row>
     <row r="142" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A142" s="12"/>
-      <c r="B142" s="15"/>
+      <c r="A142" s="13"/>
+      <c r="B142" s="14" t="s">
+        <v>219</v>
+      </c>
       <c r="C142" s="6"/>
       <c r="D142" s="4"/>
       <c r="E142" s="4"/>
@@ -4366,8 +4521,8 @@
       <c r="J142" s="4"/>
     </row>
     <row r="143" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A143" s="12"/>
-      <c r="B143" s="14"/>
+      <c r="A143" s="13"/>
+      <c r="B143" s="15"/>
       <c r="C143" s="6"/>
       <c r="D143" s="4"/>
       <c r="E143" s="4"/>
@@ -4378,10 +4533,8 @@
       <c r="J143" s="4"/>
     </row>
     <row r="144" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="12"/>
-      <c r="B144" s="13" t="s">
-        <v>222</v>
-      </c>
+      <c r="A144" s="13"/>
+      <c r="B144" s="16"/>
       <c r="C144" s="6"/>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
@@ -4392,8 +4545,10 @@
       <c r="J144" s="4"/>
     </row>
     <row r="145" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="12"/>
-      <c r="B145" s="15"/>
+      <c r="A145" s="13"/>
+      <c r="B145" s="14" t="s">
+        <v>220</v>
+      </c>
       <c r="C145" s="6"/>
       <c r="D145" s="4"/>
       <c r="E145" s="4"/>
@@ -4404,8 +4559,8 @@
       <c r="J145" s="4"/>
     </row>
     <row r="146" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A146" s="12"/>
-      <c r="B146" s="14"/>
+      <c r="A146" s="13"/>
+      <c r="B146" s="15"/>
       <c r="C146" s="6"/>
       <c r="D146" s="4"/>
       <c r="E146" s="4"/>
@@ -4415,11 +4570,8 @@
       <c r="I146" s="4"/>
       <c r="J146" s="4"/>
     </row>
-    <row r="147" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A147" s="12"/>
-      <c r="B147" s="7" t="s">
-        <v>223</v>
-      </c>
+    <row r="147" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B147" s="15"/>
       <c r="C147" s="6"/>
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
@@ -4429,11 +4581,8 @@
       <c r="I147" s="4"/>
       <c r="J147" s="4"/>
     </row>
-    <row r="148" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A148" s="12"/>
-      <c r="B148" s="13" t="s">
-        <v>224</v>
-      </c>
+    <row r="148" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B148" s="16"/>
       <c r="C148" s="6"/>
       <c r="D148" s="4"/>
       <c r="E148" s="4"/>
@@ -4443,9 +4592,10 @@
       <c r="I148" s="4"/>
       <c r="J148" s="4"/>
     </row>
-    <row r="149" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A149" s="12"/>
-      <c r="B149" s="14"/>
+    <row r="149" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B149" s="14" t="s">
+        <v>221</v>
+      </c>
       <c r="C149" s="6"/>
       <c r="D149" s="4"/>
       <c r="E149" s="4"/>
@@ -4455,27 +4605,87 @@
       <c r="I149" s="4"/>
       <c r="J149" s="4"/>
     </row>
-    <row r="150" spans="1:10" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="150" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B150" s="15"/>
+      <c r="C150" s="6"/>
+      <c r="D150" s="4"/>
+      <c r="E150" s="4"/>
+      <c r="F150" s="4"/>
+      <c r="G150" s="4"/>
+      <c r="H150" s="4"/>
+      <c r="I150" s="4"/>
+      <c r="J150" s="4"/>
+    </row>
+    <row r="151" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B151" s="16"/>
+      <c r="C151" s="6"/>
+      <c r="D151" s="4"/>
+      <c r="E151" s="4"/>
+      <c r="F151" s="4"/>
+      <c r="G151" s="4"/>
+      <c r="H151" s="4"/>
+      <c r="I151" s="4"/>
+      <c r="J151" s="4"/>
+    </row>
+    <row r="152" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B152" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C152" s="6"/>
+      <c r="D152" s="4"/>
+      <c r="E152" s="4"/>
+      <c r="F152" s="4"/>
+      <c r="G152" s="4"/>
+      <c r="H152" s="4"/>
+      <c r="I152" s="4"/>
+      <c r="J152" s="4"/>
+    </row>
+    <row r="153" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B153" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="C153" s="6"/>
+      <c r="D153" s="4"/>
+      <c r="E153" s="4"/>
+      <c r="F153" s="4"/>
+      <c r="G153" s="4"/>
+      <c r="H153" s="4"/>
+      <c r="I153" s="4"/>
+      <c r="J153" s="4"/>
+    </row>
+    <row r="154" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B154" s="16"/>
+      <c r="C154" s="6"/>
+      <c r="D154" s="4"/>
+      <c r="E154" s="4"/>
+      <c r="F154" s="4"/>
+      <c r="G154" s="4"/>
+      <c r="H154" s="4"/>
+      <c r="I154" s="4"/>
+      <c r="J154" s="4"/>
+    </row>
+    <row r="155" spans="1:10" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="B140:B143"/>
-    <mergeCell ref="B144:B146"/>
-    <mergeCell ref="A134:A149"/>
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="B16:B21"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="B27:B58"/>
-    <mergeCell ref="B59:B69"/>
-    <mergeCell ref="A2:A133"/>
-    <mergeCell ref="B148:B149"/>
-    <mergeCell ref="B70:B77"/>
-    <mergeCell ref="B78:B82"/>
-    <mergeCell ref="B83:B97"/>
-    <mergeCell ref="B98:B114"/>
-    <mergeCell ref="B115:B133"/>
-    <mergeCell ref="B134:B136"/>
-    <mergeCell ref="B137:B139"/>
+  <mergeCells count="19">
+    <mergeCell ref="B139:B141"/>
+    <mergeCell ref="B142:B144"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B145:B148"/>
+    <mergeCell ref="B149:B151"/>
+    <mergeCell ref="A131:A146"/>
+    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="B31:B63"/>
+    <mergeCell ref="B64:B74"/>
+    <mergeCell ref="A2:A130"/>
+    <mergeCell ref="B153:B154"/>
+    <mergeCell ref="B75:B82"/>
+    <mergeCell ref="B83:B87"/>
+    <mergeCell ref="B88:B102"/>
+    <mergeCell ref="B103:B119"/>
+    <mergeCell ref="B120:B138"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add geometry dfs bfs
</commit_message>
<xml_diff>
--- a/EDA_database_algorithm.xlsx
+++ b/EDA_database_algorithm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\respo\iEDA-standard-develop-codebase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F9E861-B183-422A-8A6D-3BCC4D3154EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0FA668-9C46-4890-AD2D-953CA7145FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{5A250FBF-FD77-48BD-871A-3834DD962A5A}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="239">
   <si>
     <t>EDA数据结构</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -129,851 +129,852 @@
     <t>Circle</t>
   </si>
   <si>
+    <t>Polyhedron</t>
+  </si>
+  <si>
+    <t>Line</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接口函数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cubic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Graph</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DAG（有向图）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Edge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Node</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Match</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cut</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RectangleTree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3DRectangleTree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HyperGraph</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BinaryGraph</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IntervalGraph</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>具体不展开</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>矩阵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进位制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B*Tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拓扑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OTree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列对</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2DSlot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Panel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diamond</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H Tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HV Tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SteinerTree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RectSteinerTree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3DGridGraph</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TreeGgraph</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>算法描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>输入数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>常用算法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EDA算法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DFS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BFS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Graph/Tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>双向搜索</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回溯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>深搜A*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DancingLink</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>集合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>精确覆盖问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>剪枝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动态规划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>记忆搜索</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>背包</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>区间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树形</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>矩阵乘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>矩形</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>距离</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三角剖分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>求凸包</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>扫描线</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多面体（形）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外接矩形</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>求最近点对</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>求某点范围内点集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>形状间关系</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交并补，切</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树直径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最近公共祖先</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树分割</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树合并</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拓扑排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小生成树</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小直径生成树</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第k条最短路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>连通分支</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>割点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>桥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>判断环</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小环</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图染色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平面图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>判断平面图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>欧拉路(圈)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哈密顿路(圈)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大流</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小割</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小费用流</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小费用最大流</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上下界网络流</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大匹配</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二部图最大匹配</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二部图最大权匹配</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大权匹配</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不相交路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大割划分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大独立集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小点覆盖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小边覆盖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TSP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经过固定点最短路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位运算</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>求幂</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拉格朗日插值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FFT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多项式牛顿迭代</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高斯消元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>特征多项式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单纯性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>牛顿迭代</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schreier-Sims算法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表达式求值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调度问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运筹规划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机器调度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>路径规划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>库存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>装箱问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>启发式方法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PSO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FSO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>线搜索</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>梯度方法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>共轭梯度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>内点法</t>
+  </si>
+  <si>
+    <t>拟牛顿法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有效集法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>罚/障碍/增广拉格朗日</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>椭球算法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交替方向</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机梯度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分块交替</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原始对偶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>变分法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SAT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大团</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图同构</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数值优化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>几何规划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数规划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>矩阵求导</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>矩阵变换</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>矩阵分解（QR,LU,SVD,Eigen）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>特征向量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>线性方程组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>非线性方程组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>插值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>差分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>微分方程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>边界元方法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>谱方法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拉普拉斯方程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>泊松方程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dirac算子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有限元方程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机游走</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数值计算</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数学基础</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据表达</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模型估计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>聚类</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分类</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SVM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boosting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回归</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>降维</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主动学习</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>神经网络</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>强化学习</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机森林</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贝叶斯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MCMC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自编码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>深度学习</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>广度学习</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图神经网络</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机器学习</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>逻辑综合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>物理设计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>签核分析</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>物理验证</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>版图处理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电路仿真</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一般</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>见文档</t>
+  </si>
+  <si>
+    <t>见文档</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陈英奇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>常用字符串处理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串Hash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串tire字典树</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串Kmp算法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最短路(Floyd)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最短路(dijkstra)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Polygon</t>
-  </si>
-  <si>
-    <t>Polyhedron</t>
-  </si>
-  <si>
-    <t>Line</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>接口函数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数据描述</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cubic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Graph</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DAG（有向图）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Edge</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Node</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Match</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cut</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Grid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RectangleTree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3DRectangleTree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>图</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HyperGraph</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BinaryGraph</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IntervalGraph</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>具体不展开</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数学</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>矩阵</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>张量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>向量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>进位制</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数列</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B*Tree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>序列</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>拓扑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OTree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>序列对</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Slot</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2DSlot</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Panel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Diamond</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>H Tree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HV Tree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Spine</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SteinerTree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RectSteinerTree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3DGridGraph</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TreeGgraph</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>算法描述</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>输入数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>常用算法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EDA算法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>搜索</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DFS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BFS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Graph/Tree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>双向搜索</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回溯</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>深搜A*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DancingLink</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>集合</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>精确覆盖问题</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>剪枝</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>动态规划</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>记忆搜索</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>背包</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>区间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>树形</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>矩阵乘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>矩形</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>距离</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>三角剖分</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>求凸包</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>扫描线</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>多面体（形）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>外接矩形</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>点集</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>求最近点对</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>求某点范围内点集</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>形状间关系</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>交并补，切</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>树直径</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最近公共祖先</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>路</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>树分割</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>树合并</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>拓扑排序</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最小生成树</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最小直径生成树</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第k条最短路</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>连通分支</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>割点</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>桥</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>判断环</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最小环</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>图染色</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>平面图</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>判断平面图</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>欧拉路(圈)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>哈密顿路(圈)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最大流</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最小割</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最小费用流</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最小费用最大流</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上下界网络流</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最大匹配</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>二部图最大匹配</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>二部图最大权匹配</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最大权匹配</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>不相交路</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最大割划分</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最大独立集</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最小点覆盖</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最小边覆盖</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TSP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>经过固定点最短路</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>位运算</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>求幂</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>拉格朗日插值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FFT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>多项式牛顿迭代</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>高斯消元</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>特征多项式</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>单纯性</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>牛顿迭代</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Schreier-Sims算法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表达式求值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>调度问题</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>运筹规划</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>机器调度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>路径规划</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>库存</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>装箱问题</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>启发式方法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PSO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FSO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>线搜索</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>梯度方法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>共轭梯度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>内点法</t>
-  </si>
-  <si>
-    <t>拟牛顿法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有效集法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>罚/障碍/增广拉格朗日</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>椭球算法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>交替方向</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机梯度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>分块交替</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>原始对偶</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>变分法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SAT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最大团</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>图同构</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数值优化</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>几何规划</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>整数规划</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>矩阵求导</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>矩阵变换</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>矩阵分解（QR,LU,SVD,Eigen）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>特征向量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>线性方程组</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>非线性方程组</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>插值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>差分</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>微分方程</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>边界元方法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>谱方法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>拉普拉斯方程</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>泊松方程</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dirac算子</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有限元方程</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机游走</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数值计算</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数学基础</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数据表达</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>模型估计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>聚类</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>分类</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SVM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Boosting</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回归</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>排序</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>降维</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>主动学习</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>神经网络</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>强化学习</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机森林</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>贝叶斯</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MCMC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>自编码</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>深度学习</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>广度学习</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>图神经网络</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>机器学习</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>逻辑综合</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>物理设计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>签核分析</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>物理验证</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>版图处理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>电路仿真</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成日期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>已完成</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一般</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>见文档</t>
-  </si>
-  <si>
-    <t>见文档</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>陈英奇</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>字符串</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>常用字符串处理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>字符串Hash</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>字符串tire字典树</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>字符串Kmp算法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最短路(Floyd)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最短路(dijkstra)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1166,10 +1167,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1490,7 +1491,7 @@
   <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1514,10 +1515,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1529,7 +1530,7 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -1541,7 +1542,7 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -1556,25 +1557,25 @@
         <v>13</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>230</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>231</v>
       </c>
       <c r="I3" s="12">
         <v>44472</v>
@@ -1588,19 +1589,19 @@
         <v>9</v>
       </c>
       <c r="D4" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>230</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>231</v>
       </c>
       <c r="I4" s="12">
         <v>44473</v>
@@ -1614,19 +1615,19 @@
         <v>10</v>
       </c>
       <c r="D5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>230</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>231</v>
       </c>
       <c r="I5" s="12">
         <v>44472</v>
@@ -1642,19 +1643,19 @@
         <v>11</v>
       </c>
       <c r="D6" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>230</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>231</v>
       </c>
       <c r="I6" s="12">
         <v>44475</v>
@@ -1668,19 +1669,19 @@
         <v>12</v>
       </c>
       <c r="D7" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>230</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>231</v>
       </c>
       <c r="I7" s="12">
         <v>44475</v>
@@ -1694,19 +1695,19 @@
         <v>15</v>
       </c>
       <c r="D8" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>230</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>231</v>
       </c>
       <c r="I8" s="12">
         <v>44483</v>
@@ -1720,19 +1721,19 @@
         <v>16</v>
       </c>
       <c r="D9" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>230</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>231</v>
       </c>
       <c r="I9" s="12">
         <v>44492</v>
@@ -1757,7 +1758,7 @@
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1771,7 +1772,7 @@
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1800,44 +1801,80 @@
       <c r="B14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
+      <c r="D14" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="I14" s="12">
+        <v>44509</v>
+      </c>
+      <c r="J14" s="11"/>
     </row>
     <row r="15" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
-      <c r="C15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
+      <c r="C15" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="I15" s="12">
+        <v>44509</v>
+      </c>
+      <c r="J15" s="11"/>
     </row>
     <row r="16" spans="1:10" ht="15.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
+      <c r="D16" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="I16" s="12">
+        <v>44509</v>
+      </c>
+      <c r="J16" s="11"/>
     </row>
     <row r="17" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13"/>
@@ -1870,22 +1907,34 @@
     <row r="19" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
-      <c r="C19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="C19" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="I19" s="12">
+        <v>44509</v>
+      </c>
+      <c r="J19" s="11"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
       <c r="C20" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -1899,7 +1948,7 @@
       <c r="A21" s="13"/>
       <c r="B21" s="13"/>
       <c r="C21" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -1912,10 +1961,10 @@
     <row r="22" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13"/>
       <c r="B22" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -1929,7 +1978,7 @@
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -1943,7 +1992,7 @@
       <c r="A24" s="13"/>
       <c r="B24" s="13"/>
       <c r="C24" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -1957,7 +2006,7 @@
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1971,7 +2020,7 @@
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -1985,7 +2034,7 @@
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -1999,7 +2048,7 @@
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -2013,7 +2062,7 @@
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -2027,7 +2076,7 @@
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -2041,7 +2090,7 @@
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -2055,7 +2104,7 @@
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -2069,7 +2118,7 @@
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -2082,10 +2131,10 @@
     <row r="34" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
       <c r="B34" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -2099,7 +2148,7 @@
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -2113,7 +2162,7 @@
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -2127,7 +2176,7 @@
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -2141,7 +2190,7 @@
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -2156,10 +2205,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -2175,7 +2224,7 @@
         <v>20</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -2189,7 +2238,7 @@
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -2203,7 +2252,7 @@
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -2217,7 +2266,7 @@
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -2231,7 +2280,7 @@
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -2245,7 +2294,7 @@
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -2258,10 +2307,10 @@
     <row r="46" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="13"/>
       <c r="B46" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -2275,7 +2324,7 @@
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
       <c r="C47" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
@@ -2289,7 +2338,7 @@
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -2303,7 +2352,7 @@
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -2317,7 +2366,7 @@
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -2331,7 +2380,7 @@
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -2364,8 +2413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1B1B9C-0591-4BED-8FBD-040911B92B66}">
   <dimension ref="A1:J155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2389,10 +2438,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -2412,28 +2461,28 @@
     </row>
     <row r="2" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>233</v>
-      </c>
       <c r="D2" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>230</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>231</v>
       </c>
       <c r="I2" s="12">
         <v>44444</v>
@@ -2442,24 +2491,24 @@
     </row>
     <row r="3" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
-      <c r="B3" s="15"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D3" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>230</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>231</v>
       </c>
       <c r="I3" s="12">
         <v>44449</v>
@@ -2468,24 +2517,24 @@
     </row>
     <row r="4" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13"/>
-      <c r="B4" s="15"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D4" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>230</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>231</v>
       </c>
       <c r="I4" s="12">
         <v>44455</v>
@@ -2494,24 +2543,24 @@
     </row>
     <row r="5" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>
-      <c r="B5" s="15"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D5" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>230</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>231</v>
       </c>
       <c r="I5" s="12">
         <v>44468</v>
@@ -2521,46 +2570,62 @@
     <row r="6" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13"/>
       <c r="B6" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="I6" s="12">
+        <v>44509</v>
+      </c>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="F7" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="I7" s="12">
+        <v>44509</v>
+      </c>
+      <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -2572,11 +2637,11 @@
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -2588,11 +2653,11 @@
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
       <c r="C10" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -2604,11 +2669,11 @@
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -2620,13 +2685,13 @@
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -2638,11 +2703,11 @@
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -2653,10 +2718,10 @@
     <row r="14" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13"/>
       <c r="B14" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -2670,7 +2735,7 @@
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -2684,7 +2749,7 @@
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
       <c r="C16" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -2698,7 +2763,7 @@
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
       <c r="C17" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
@@ -2714,7 +2779,7 @@
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -2728,7 +2793,7 @@
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
       <c r="C19" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -2744,13 +2809,13 @@
         <v>21</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>103</v>
-      </c>
       <c r="E20" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -2762,11 +2827,11 @@
       <c r="A21" s="13"/>
       <c r="B21" s="13"/>
       <c r="C21" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -2778,11 +2843,11 @@
       <c r="A22" s="13"/>
       <c r="B22" s="13"/>
       <c r="C22" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -2794,11 +2859,11 @@
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -2810,11 +2875,11 @@
       <c r="A24" s="13"/>
       <c r="B24" s="13"/>
       <c r="C24" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -2826,11 +2891,11 @@
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -2844,7 +2909,7 @@
         <v>20</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -2858,22 +2923,22 @@
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D27" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H27" s="11" t="s">
         <v>230</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>231</v>
       </c>
       <c r="I27" s="12">
         <v>44494</v>
@@ -2884,7 +2949,7 @@
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -2898,7 +2963,7 @@
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -2912,7 +2977,7 @@
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -2925,10 +2990,10 @@
     <row r="31" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="13"/>
       <c r="B31" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -2942,7 +3007,7 @@
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -2956,7 +3021,7 @@
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -2970,22 +3035,22 @@
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D34" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H34" s="11" t="s">
         <v>230</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="H34" s="11" t="s">
-        <v>231</v>
       </c>
       <c r="I34" s="12">
         <v>44471</v>
@@ -2996,22 +3061,22 @@
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D35" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H35" s="11" t="s">
         <v>230</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>231</v>
       </c>
       <c r="I35" s="12">
         <v>44471</v>
@@ -3022,7 +3087,7 @@
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -3036,7 +3101,7 @@
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -3050,7 +3115,7 @@
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -3064,7 +3129,7 @@
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -3078,7 +3143,7 @@
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -3092,7 +3157,7 @@
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -3106,7 +3171,7 @@
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -3120,7 +3185,7 @@
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -3134,7 +3199,7 @@
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -3148,7 +3213,7 @@
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -3162,7 +3227,7 @@
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -3176,7 +3241,7 @@
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
       <c r="C47" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
@@ -3190,7 +3255,7 @@
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -3204,7 +3269,7 @@
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -3218,7 +3283,7 @@
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -3232,7 +3297,7 @@
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -3246,7 +3311,7 @@
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -3260,7 +3325,7 @@
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
       <c r="C53" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -3274,7 +3339,7 @@
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -3288,7 +3353,7 @@
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -3302,7 +3367,7 @@
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
@@ -3316,7 +3381,7 @@
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="C57" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
@@ -3330,7 +3395,7 @@
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
@@ -3344,7 +3409,7 @@
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
@@ -3358,7 +3423,7 @@
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
@@ -3372,7 +3437,7 @@
       <c r="A61" s="13"/>
       <c r="B61" s="13"/>
       <c r="C61" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -3386,7 +3451,7 @@
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
@@ -3400,7 +3465,7 @@
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="C63" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
@@ -3413,14 +3478,14 @@
     <row r="64" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="13"/>
       <c r="B64" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -3432,11 +3497,11 @@
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
       <c r="C65" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
@@ -3448,7 +3513,7 @@
       <c r="A66" s="13"/>
       <c r="B66" s="13"/>
       <c r="C66" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
@@ -3462,7 +3527,7 @@
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
       <c r="C67" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
@@ -3476,7 +3541,7 @@
       <c r="A68" s="13"/>
       <c r="B68" s="13"/>
       <c r="C68" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
@@ -3490,7 +3555,7 @@
       <c r="A69" s="13"/>
       <c r="B69" s="13"/>
       <c r="C69" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
@@ -3504,7 +3569,7 @@
       <c r="A70" s="13"/>
       <c r="B70" s="13"/>
       <c r="C70" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
@@ -3518,7 +3583,7 @@
       <c r="A71" s="13"/>
       <c r="B71" s="13"/>
       <c r="C71" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
@@ -3532,7 +3597,7 @@
       <c r="A72" s="13"/>
       <c r="B72" s="13"/>
       <c r="C72" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
@@ -3546,7 +3611,7 @@
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
       <c r="C73" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
@@ -3560,7 +3625,7 @@
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="C74" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -3573,10 +3638,10 @@
     <row r="75" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="13"/>
       <c r="B75" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
@@ -3590,7 +3655,7 @@
       <c r="A76" s="13"/>
       <c r="B76" s="13"/>
       <c r="C76" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -3604,7 +3669,7 @@
       <c r="A77" s="13"/>
       <c r="B77" s="13"/>
       <c r="C77" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
@@ -3618,7 +3683,7 @@
       <c r="A78" s="13"/>
       <c r="B78" s="13"/>
       <c r="C78" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
@@ -3632,7 +3697,7 @@
       <c r="A79" s="13"/>
       <c r="B79" s="13"/>
       <c r="C79" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
@@ -3646,7 +3711,7 @@
       <c r="A80" s="13"/>
       <c r="B80" s="13"/>
       <c r="C80" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
@@ -3660,7 +3725,7 @@
       <c r="A81" s="13"/>
       <c r="B81" s="13"/>
       <c r="C81" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
@@ -3674,7 +3739,7 @@
       <c r="A82" s="13"/>
       <c r="B82" s="13"/>
       <c r="C82" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
@@ -3687,10 +3752,10 @@
     <row r="83" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="13"/>
       <c r="B83" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C83" s="6" t="s">
         <v>156</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>157</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="4"/>
@@ -3704,7 +3769,7 @@
       <c r="A84" s="13"/>
       <c r="B84" s="13"/>
       <c r="C84" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
@@ -3718,7 +3783,7 @@
       <c r="A85" s="13"/>
       <c r="B85" s="13"/>
       <c r="C85" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
@@ -3732,7 +3797,7 @@
       <c r="A86" s="13"/>
       <c r="B86" s="13"/>
       <c r="C86" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
@@ -3746,7 +3811,7 @@
       <c r="A87" s="13"/>
       <c r="B87" s="13"/>
       <c r="C87" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -3759,10 +3824,10 @@
     <row r="88" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="13"/>
       <c r="B88" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
@@ -3776,7 +3841,7 @@
       <c r="A89" s="13"/>
       <c r="B89" s="13"/>
       <c r="C89" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
@@ -3790,7 +3855,7 @@
       <c r="A90" s="13"/>
       <c r="B90" s="13"/>
       <c r="C90" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
@@ -3804,7 +3869,7 @@
       <c r="A91" s="13"/>
       <c r="B91" s="13"/>
       <c r="C91" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
@@ -3818,7 +3883,7 @@
       <c r="A92" s="13"/>
       <c r="B92" s="13"/>
       <c r="C92" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
@@ -3832,7 +3897,7 @@
       <c r="A93" s="13"/>
       <c r="B93" s="13"/>
       <c r="C93" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
@@ -3846,7 +3911,7 @@
       <c r="A94" s="13"/>
       <c r="B94" s="13"/>
       <c r="C94" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
@@ -3860,7 +3925,7 @@
       <c r="A95" s="13"/>
       <c r="B95" s="13"/>
       <c r="C95" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4"/>
@@ -3874,7 +3939,7 @@
       <c r="A96" s="13"/>
       <c r="B96" s="13"/>
       <c r="C96" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
@@ -3888,7 +3953,7 @@
       <c r="A97" s="13"/>
       <c r="B97" s="13"/>
       <c r="C97" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
@@ -3902,7 +3967,7 @@
       <c r="A98" s="13"/>
       <c r="B98" s="13"/>
       <c r="C98" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
@@ -3916,7 +3981,7 @@
       <c r="A99" s="13"/>
       <c r="B99" s="13"/>
       <c r="C99" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
@@ -3930,7 +3995,7 @@
       <c r="A100" s="13"/>
       <c r="B100" s="13"/>
       <c r="C100" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
@@ -3944,7 +4009,7 @@
       <c r="A101" s="13"/>
       <c r="B101" s="13"/>
       <c r="C101" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>
@@ -3958,7 +4023,7 @@
       <c r="A102" s="13"/>
       <c r="B102" s="13"/>
       <c r="C102" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="4"/>
@@ -3971,10 +4036,10 @@
     <row r="103" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="13"/>
       <c r="B103" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="4"/>
@@ -3988,7 +4053,7 @@
       <c r="A104" s="13"/>
       <c r="B104" s="13"/>
       <c r="C104" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D104" s="4"/>
       <c r="E104" s="4"/>
@@ -4002,7 +4067,7 @@
       <c r="A105" s="13"/>
       <c r="B105" s="13"/>
       <c r="C105" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D105" s="4"/>
       <c r="E105" s="4"/>
@@ -4016,7 +4081,7 @@
       <c r="A106" s="13"/>
       <c r="B106" s="13"/>
       <c r="C106" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D106" s="4"/>
       <c r="E106" s="4"/>
@@ -4030,7 +4095,7 @@
       <c r="A107" s="13"/>
       <c r="B107" s="13"/>
       <c r="C107" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
@@ -4044,7 +4109,7 @@
       <c r="A108" s="13"/>
       <c r="B108" s="13"/>
       <c r="C108" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D108" s="4"/>
       <c r="E108" s="4"/>
@@ -4058,7 +4123,7 @@
       <c r="A109" s="13"/>
       <c r="B109" s="13"/>
       <c r="C109" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
@@ -4072,7 +4137,7 @@
       <c r="A110" s="13"/>
       <c r="B110" s="13"/>
       <c r="C110" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
@@ -4086,7 +4151,7 @@
       <c r="A111" s="13"/>
       <c r="B111" s="13"/>
       <c r="C111" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
@@ -4100,7 +4165,7 @@
       <c r="A112" s="13"/>
       <c r="B112" s="13"/>
       <c r="C112" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
@@ -4114,7 +4179,7 @@
       <c r="A113" s="13"/>
       <c r="B113" s="13"/>
       <c r="C113" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
@@ -4128,7 +4193,7 @@
       <c r="A114" s="13"/>
       <c r="B114" s="13"/>
       <c r="C114" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D114" s="4"/>
       <c r="E114" s="4"/>
@@ -4142,7 +4207,7 @@
       <c r="A115" s="13"/>
       <c r="B115" s="13"/>
       <c r="C115" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
@@ -4156,7 +4221,7 @@
       <c r="A116" s="13"/>
       <c r="B116" s="13"/>
       <c r="C116" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
@@ -4170,7 +4235,7 @@
       <c r="A117" s="13"/>
       <c r="B117" s="13"/>
       <c r="C117" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
@@ -4184,7 +4249,7 @@
       <c r="A118" s="13"/>
       <c r="B118" s="13"/>
       <c r="C118" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
@@ -4198,7 +4263,7 @@
       <c r="A119" s="13"/>
       <c r="B119" s="13"/>
       <c r="C119" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
@@ -4211,10 +4276,10 @@
     <row r="120" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="13"/>
       <c r="B120" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D120" s="4"/>
       <c r="E120" s="4"/>
@@ -4228,7 +4293,7 @@
       <c r="A121" s="13"/>
       <c r="B121" s="13"/>
       <c r="C121" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
@@ -4242,7 +4307,7 @@
       <c r="A122" s="13"/>
       <c r="B122" s="13"/>
       <c r="C122" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D122" s="4"/>
       <c r="E122" s="4"/>
@@ -4256,7 +4321,7 @@
       <c r="A123" s="13"/>
       <c r="B123" s="13"/>
       <c r="C123" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D123" s="4"/>
       <c r="E123" s="4"/>
@@ -4270,7 +4335,7 @@
       <c r="A124" s="13"/>
       <c r="B124" s="13"/>
       <c r="C124" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D124" s="4"/>
       <c r="E124" s="4"/>
@@ -4284,7 +4349,7 @@
       <c r="A125" s="13"/>
       <c r="B125" s="13"/>
       <c r="C125" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="4"/>
@@ -4298,7 +4363,7 @@
       <c r="A126" s="13"/>
       <c r="B126" s="13"/>
       <c r="C126" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D126" s="4"/>
       <c r="E126" s="4"/>
@@ -4312,7 +4377,7 @@
       <c r="A127" s="13"/>
       <c r="B127" s="13"/>
       <c r="C127" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D127" s="4"/>
       <c r="E127" s="4"/>
@@ -4326,7 +4391,7 @@
       <c r="A128" s="13"/>
       <c r="B128" s="13"/>
       <c r="C128" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D128" s="4"/>
       <c r="E128" s="4"/>
@@ -4340,7 +4405,7 @@
       <c r="A129" s="13"/>
       <c r="B129" s="13"/>
       <c r="C129" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D129" s="4"/>
       <c r="E129" s="4"/>
@@ -4354,7 +4419,7 @@
       <c r="A130" s="13"/>
       <c r="B130" s="13"/>
       <c r="C130" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D130" s="4"/>
       <c r="E130" s="4"/>
@@ -4366,11 +4431,11 @@
     </row>
     <row r="131" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B131" s="13"/>
       <c r="C131" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D131" s="4"/>
       <c r="E131" s="4"/>
@@ -4384,7 +4449,7 @@
       <c r="A132" s="13"/>
       <c r="B132" s="13"/>
       <c r="C132" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D132" s="4"/>
       <c r="E132" s="4"/>
@@ -4398,7 +4463,7 @@
       <c r="A133" s="13"/>
       <c r="B133" s="13"/>
       <c r="C133" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="4"/>
@@ -4412,7 +4477,7 @@
       <c r="A134" s="13"/>
       <c r="B134" s="13"/>
       <c r="C134" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D134" s="4"/>
       <c r="E134" s="4"/>
@@ -4426,7 +4491,7 @@
       <c r="A135" s="13"/>
       <c r="B135" s="13"/>
       <c r="C135" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D135" s="4"/>
       <c r="E135" s="4"/>
@@ -4440,7 +4505,7 @@
       <c r="A136" s="13"/>
       <c r="B136" s="13"/>
       <c r="C136" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D136" s="4"/>
       <c r="E136" s="4"/>
@@ -4454,7 +4519,7 @@
       <c r="A137" s="13"/>
       <c r="B137" s="13"/>
       <c r="C137" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
@@ -4468,7 +4533,7 @@
       <c r="A138" s="13"/>
       <c r="B138" s="13"/>
       <c r="C138" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D138" s="4"/>
       <c r="E138" s="4"/>
@@ -4481,10 +4546,10 @@
     <row r="139" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A139" s="13"/>
       <c r="B139" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="C139" s="6" t="s">
         <v>224</v>
-      </c>
-      <c r="C139" s="6" t="s">
-        <v>225</v>
       </c>
       <c r="D139" s="4"/>
       <c r="E139" s="4"/>
@@ -4496,7 +4561,7 @@
     </row>
     <row r="140" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="13"/>
-      <c r="B140" s="15"/>
+      <c r="B140" s="16"/>
       <c r="C140" s="6"/>
       <c r="D140" s="4"/>
       <c r="E140" s="4"/>
@@ -4508,7 +4573,7 @@
     </row>
     <row r="141" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="13"/>
-      <c r="B141" s="16"/>
+      <c r="B141" s="15"/>
       <c r="C141" s="6"/>
       <c r="D141" s="4"/>
       <c r="E141" s="4"/>
@@ -4521,7 +4586,7 @@
     <row r="142" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="13"/>
       <c r="B142" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C142" s="6"/>
       <c r="D142" s="4"/>
@@ -4534,7 +4599,7 @@
     </row>
     <row r="143" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="13"/>
-      <c r="B143" s="15"/>
+      <c r="B143" s="16"/>
       <c r="C143" s="6"/>
       <c r="D143" s="4"/>
       <c r="E143" s="4"/>
@@ -4546,7 +4611,7 @@
     </row>
     <row r="144" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="13"/>
-      <c r="B144" s="16"/>
+      <c r="B144" s="15"/>
       <c r="C144" s="6"/>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
@@ -4559,7 +4624,7 @@
     <row r="145" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="13"/>
       <c r="B145" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C145" s="6"/>
       <c r="D145" s="4"/>
@@ -4572,7 +4637,7 @@
     </row>
     <row r="146" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="13"/>
-      <c r="B146" s="15"/>
+      <c r="B146" s="16"/>
       <c r="C146" s="6"/>
       <c r="D146" s="4"/>
       <c r="E146" s="4"/>
@@ -4583,7 +4648,7 @@
       <c r="J146" s="4"/>
     </row>
     <row r="147" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B147" s="15"/>
+      <c r="B147" s="16"/>
       <c r="C147" s="6"/>
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
@@ -4594,7 +4659,7 @@
       <c r="J147" s="4"/>
     </row>
     <row r="148" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B148" s="16"/>
+      <c r="B148" s="15"/>
       <c r="C148" s="6"/>
       <c r="D148" s="4"/>
       <c r="E148" s="4"/>
@@ -4606,7 +4671,7 @@
     </row>
     <row r="149" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B149" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C149" s="6"/>
       <c r="D149" s="4"/>
@@ -4618,7 +4683,7 @@
       <c r="J149" s="4"/>
     </row>
     <row r="150" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B150" s="15"/>
+      <c r="B150" s="16"/>
       <c r="C150" s="6"/>
       <c r="D150" s="4"/>
       <c r="E150" s="4"/>
@@ -4629,7 +4694,7 @@
       <c r="J150" s="4"/>
     </row>
     <row r="151" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B151" s="16"/>
+      <c r="B151" s="15"/>
       <c r="C151" s="6"/>
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
@@ -4641,7 +4706,7 @@
     </row>
     <row r="152" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B152" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C152" s="6"/>
       <c r="D152" s="4"/>
@@ -4654,7 +4719,7 @@
     </row>
     <row r="153" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B153" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C153" s="6"/>
       <c r="D153" s="4"/>
@@ -4666,7 +4731,7 @@
       <c r="J153" s="4"/>
     </row>
     <row r="154" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B154" s="16"/>
+      <c r="B154" s="15"/>
       <c r="C154" s="6"/>
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
@@ -4679,12 +4744,6 @@
     <row r="155" spans="1:10" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B153:B154"/>
-    <mergeCell ref="B75:B82"/>
-    <mergeCell ref="B83:B87"/>
-    <mergeCell ref="B88:B102"/>
-    <mergeCell ref="B103:B119"/>
-    <mergeCell ref="B120:B138"/>
     <mergeCell ref="A131:A146"/>
     <mergeCell ref="B6:B13"/>
     <mergeCell ref="B14:B19"/>
@@ -4697,6 +4756,12 @@
     <mergeCell ref="B142:B144"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B145:B148"/>
+    <mergeCell ref="B153:B154"/>
+    <mergeCell ref="B75:B82"/>
+    <mergeCell ref="B83:B87"/>
+    <mergeCell ref="B88:B102"/>
+    <mergeCell ref="B103:B119"/>
+    <mergeCell ref="B120:B138"/>
     <mergeCell ref="B149:B151"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add cut and flow
</commit_message>
<xml_diff>
--- a/EDA_database_algorithm.xlsx
+++ b/EDA_database_algorithm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pcl\standard_develop\iEDA-standard-develop-codebase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43EEDA7-FC39-4DF1-84E4-A02712F0276E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5E2F0E-E8D6-4343-A485-EF1042D3912E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" activeTab="1" xr2:uid="{5A250FBF-FD77-48BD-871A-3834DD962A5A}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="239">
   <si>
     <t>EDA数据结构</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1167,10 +1167,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2413,8 +2413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1B1B9C-0591-4BED-8FBD-040911B92B66}">
   <dimension ref="A1:J155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2491,7 +2491,7 @@
     </row>
     <row r="3" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
-      <c r="B3" s="15"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="11" t="s">
         <v>233</v>
       </c>
@@ -2517,7 +2517,7 @@
     </row>
     <row r="4" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13"/>
-      <c r="B4" s="15"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="11" t="s">
         <v>234</v>
       </c>
@@ -2543,7 +2543,7 @@
     </row>
     <row r="5" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>
-      <c r="B5" s="15"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="11" t="s">
         <v>235</v>
       </c>
@@ -3334,30 +3334,54 @@
     <row r="47" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
+      <c r="D47" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H47" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="I47" s="12">
+        <v>44535</v>
+      </c>
+      <c r="J47" s="12"/>
     </row>
     <row r="48" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
+      <c r="D48" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H48" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="I48" s="12">
+        <v>44535</v>
+      </c>
+      <c r="J48" s="12"/>
     </row>
     <row r="49" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="13"/>
@@ -4679,7 +4703,7 @@
     </row>
     <row r="140" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="13"/>
-      <c r="B140" s="15"/>
+      <c r="B140" s="16"/>
       <c r="C140" s="6"/>
       <c r="D140" s="4"/>
       <c r="E140" s="4"/>
@@ -4691,7 +4715,7 @@
     </row>
     <row r="141" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="13"/>
-      <c r="B141" s="16"/>
+      <c r="B141" s="15"/>
       <c r="C141" s="6"/>
       <c r="D141" s="4"/>
       <c r="E141" s="4"/>
@@ -4717,7 +4741,7 @@
     </row>
     <row r="143" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="13"/>
-      <c r="B143" s="15"/>
+      <c r="B143" s="16"/>
       <c r="C143" s="6"/>
       <c r="D143" s="4"/>
       <c r="E143" s="4"/>
@@ -4729,7 +4753,7 @@
     </row>
     <row r="144" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="13"/>
-      <c r="B144" s="16"/>
+      <c r="B144" s="15"/>
       <c r="C144" s="6"/>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
@@ -4755,7 +4779,7 @@
     </row>
     <row r="146" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="13"/>
-      <c r="B146" s="15"/>
+      <c r="B146" s="16"/>
       <c r="C146" s="6"/>
       <c r="D146" s="4"/>
       <c r="E146" s="4"/>
@@ -4766,7 +4790,7 @@
       <c r="J146" s="4"/>
     </row>
     <row r="147" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B147" s="15"/>
+      <c r="B147" s="16"/>
       <c r="C147" s="6"/>
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
@@ -4777,7 +4801,7 @@
       <c r="J147" s="4"/>
     </row>
     <row r="148" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B148" s="16"/>
+      <c r="B148" s="15"/>
       <c r="C148" s="6"/>
       <c r="D148" s="4"/>
       <c r="E148" s="4"/>
@@ -4801,7 +4825,7 @@
       <c r="J149" s="4"/>
     </row>
     <row r="150" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B150" s="15"/>
+      <c r="B150" s="16"/>
       <c r="C150" s="6"/>
       <c r="D150" s="4"/>
       <c r="E150" s="4"/>
@@ -4812,7 +4836,7 @@
       <c r="J150" s="4"/>
     </row>
     <row r="151" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B151" s="16"/>
+      <c r="B151" s="15"/>
       <c r="C151" s="6"/>
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
@@ -4849,7 +4873,7 @@
       <c r="J153" s="4"/>
     </row>
     <row r="154" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B154" s="16"/>
+      <c r="B154" s="15"/>
       <c r="C154" s="6"/>
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
@@ -4862,13 +4886,6 @@
     <row r="155" spans="1:10" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B153:B154"/>
-    <mergeCell ref="B75:B82"/>
-    <mergeCell ref="B83:B87"/>
-    <mergeCell ref="B88:B102"/>
-    <mergeCell ref="B103:B119"/>
-    <mergeCell ref="B120:B138"/>
-    <mergeCell ref="B149:B151"/>
     <mergeCell ref="A131:A146"/>
     <mergeCell ref="B6:B13"/>
     <mergeCell ref="B14:B19"/>
@@ -4881,6 +4898,13 @@
     <mergeCell ref="B142:B144"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B145:B148"/>
+    <mergeCell ref="B153:B154"/>
+    <mergeCell ref="B75:B82"/>
+    <mergeCell ref="B83:B87"/>
+    <mergeCell ref="B88:B102"/>
+    <mergeCell ref="B103:B119"/>
+    <mergeCell ref="B120:B138"/>
+    <mergeCell ref="B149:B151"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update red black tree
</commit_message>
<xml_diff>
--- a/EDA_database_algorithm.xlsx
+++ b/EDA_database_algorithm.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\respo\iEDA-standard-develop-codebase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pcl\standard_develop\iEDA-standard-develop-codebase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A57A37-5995-4E81-90EE-1437B1EB989E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BE5848-AB8A-4AAF-AD02-4644D38C6738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10290" yWindow="6500" windowWidth="28800" windowHeight="15460" activeTab="1" xr2:uid="{5A250FBF-FD77-48BD-871A-3834DD962A5A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{5A250FBF-FD77-48BD-871A-3834DD962A5A}"/>
   </bookViews>
   <sheets>
     <sheet name="数据结构" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="240">
   <si>
     <t>EDA数据结构</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -975,6 +975,10 @@
   </si>
   <si>
     <t>Polygon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红黑树</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1167,10 +1171,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1488,10 +1492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7543B24A-7FB2-4879-9E7B-EB413EED23FE}">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1743,22 +1747,34 @@
     <row r="10" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
-      <c r="C10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
+      <c r="C10" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="I10" s="12">
+        <v>44591</v>
+      </c>
+      <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="4" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1772,7 +1788,7 @@
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1786,7 +1802,7 @@
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="4" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -1798,37 +1814,25 @@
     </row>
     <row r="14" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13"/>
-      <c r="B14" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="I14" s="12">
-        <v>44509</v>
-      </c>
-      <c r="J14" s="11"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
+      <c r="B15" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="C15" s="11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>229</v>
@@ -1850,11 +1854,11 @@
       </c>
       <c r="J15" s="11"/>
     </row>
-    <row r="16" spans="1:10" ht="15.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
       <c r="C16" s="11" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>229</v>
@@ -1876,25 +1880,37 @@
       </c>
       <c r="J16" s="11"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
-      <c r="C17" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
+      <c r="C17" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="I17" s="12">
+        <v>44509</v>
+      </c>
+      <c r="J17" s="11"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -1907,48 +1923,48 @@
     <row r="19" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
-      <c r="C19" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="I19" s="12">
-        <v>44509</v>
-      </c>
-      <c r="J19" s="11"/>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
-      <c r="C20" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="I20" s="12">
+        <v>44509</v>
+      </c>
+      <c r="J20" s="11"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
       <c r="B21" s="13"/>
       <c r="C21" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -1960,11 +1976,9 @@
     </row>
     <row r="22" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13"/>
-      <c r="B22" s="13" t="s">
-        <v>41</v>
-      </c>
+      <c r="B22" s="13"/>
       <c r="C22" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -1976,9 +1990,11 @@
     </row>
     <row r="23" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
+      <c r="B23" s="13" t="s">
+        <v>41</v>
+      </c>
       <c r="C23" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -1992,7 +2008,7 @@
       <c r="A24" s="13"/>
       <c r="B24" s="13"/>
       <c r="C24" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -2006,7 +2022,7 @@
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -2020,7 +2036,7 @@
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -2034,7 +2050,7 @@
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -2044,11 +2060,11 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:10" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -2058,11 +2074,11 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -2076,7 +2092,7 @@
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -2090,7 +2106,7 @@
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="6" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -2104,7 +2120,7 @@
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="6" t="s">
-        <v>118</v>
+        <v>37</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -2118,7 +2134,7 @@
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="6" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -2130,11 +2146,9 @@
     </row>
     <row r="34" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
-      <c r="B34" s="13" t="s">
-        <v>46</v>
-      </c>
+      <c r="B34" s="13"/>
       <c r="C34" s="6" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -2146,9 +2160,11 @@
     </row>
     <row r="35" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
+      <c r="B35" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="C35" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -2162,7 +2178,7 @@
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -2176,7 +2192,7 @@
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -2190,7 +2206,7 @@
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -2201,14 +2217,10 @@
       <c r="J38" s="4"/>
     </row>
     <row r="39" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
       <c r="C39" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -2219,12 +2231,14 @@
       <c r="J39" s="4"/>
     </row>
     <row r="40" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13" t="s">
-        <v>20</v>
+      <c r="A40" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -2236,9 +2250,11 @@
     </row>
     <row r="41" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
+      <c r="B41" s="13" t="s">
+        <v>20</v>
+      </c>
       <c r="C41" s="6" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -2252,7 +2268,7 @@
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -2266,7 +2282,7 @@
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -2276,11 +2292,11 @@
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
     </row>
-    <row r="44" spans="1:10" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -2290,11 +2306,11 @@
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
     </row>
-    <row r="45" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -2306,11 +2322,9 @@
     </row>
     <row r="46" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="13"/>
-      <c r="B46" s="13" t="s">
-        <v>54</v>
-      </c>
+      <c r="B46" s="13"/>
       <c r="C46" s="6" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -2322,9 +2336,11 @@
     </row>
     <row r="47" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="13"/>
-      <c r="B47" s="13"/>
+      <c r="B47" s="13" t="s">
+        <v>54</v>
+      </c>
       <c r="C47" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
@@ -2338,7 +2354,7 @@
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -2352,7 +2368,7 @@
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -2366,7 +2382,7 @@
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -2380,7 +2396,7 @@
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -2390,17 +2406,31 @@
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
     </row>
-    <row r="52" spans="1:10" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="13"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+    </row>
+    <row r="53" spans="1:10" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A39:A51"/>
-    <mergeCell ref="B40:B45"/>
-    <mergeCell ref="B46:B51"/>
-    <mergeCell ref="B6:B13"/>
-    <mergeCell ref="B14:B21"/>
-    <mergeCell ref="B22:B33"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="A3:A38"/>
+    <mergeCell ref="A40:A52"/>
+    <mergeCell ref="B41:B46"/>
+    <mergeCell ref="B47:B52"/>
+    <mergeCell ref="B6:B14"/>
+    <mergeCell ref="B15:B22"/>
+    <mergeCell ref="B23:B34"/>
+    <mergeCell ref="B35:B39"/>
+    <mergeCell ref="A3:A39"/>
     <mergeCell ref="B3:B5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2413,8 +2443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1B1B9C-0591-4BED-8FBD-040911B92B66}">
   <dimension ref="A1:J155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2491,7 +2521,7 @@
     </row>
     <row r="3" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
-      <c r="B3" s="16"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="11" t="s">
         <v>233</v>
       </c>
@@ -2517,7 +2547,7 @@
     </row>
     <row r="4" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13"/>
-      <c r="B4" s="16"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="11" t="s">
         <v>234</v>
       </c>
@@ -2543,7 +2573,7 @@
     </row>
     <row r="5" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>
-      <c r="B5" s="16"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="11" t="s">
         <v>235</v>
       </c>
@@ -3332,15 +3362,27 @@
     <row r="39" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
+      <c r="D39" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="I39" s="12">
+        <v>44592</v>
+      </c>
       <c r="J39" s="4"/>
     </row>
     <row r="40" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3360,15 +3402,27 @@
     <row r="41" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
+      <c r="D41" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="I41" s="12">
+        <v>44592</v>
+      </c>
       <c r="J41" s="4"/>
     </row>
     <row r="42" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4813,7 +4867,7 @@
     </row>
     <row r="140" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="13"/>
-      <c r="B140" s="16"/>
+      <c r="B140" s="15"/>
       <c r="C140" s="6"/>
       <c r="D140" s="4"/>
       <c r="E140" s="4"/>
@@ -4825,7 +4879,7 @@
     </row>
     <row r="141" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="13"/>
-      <c r="B141" s="15"/>
+      <c r="B141" s="16"/>
       <c r="C141" s="6"/>
       <c r="D141" s="4"/>
       <c r="E141" s="4"/>
@@ -4851,7 +4905,7 @@
     </row>
     <row r="143" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="13"/>
-      <c r="B143" s="16"/>
+      <c r="B143" s="15"/>
       <c r="C143" s="6"/>
       <c r="D143" s="4"/>
       <c r="E143" s="4"/>
@@ -4863,7 +4917,7 @@
     </row>
     <row r="144" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="13"/>
-      <c r="B144" s="15"/>
+      <c r="B144" s="16"/>
       <c r="C144" s="6"/>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
@@ -4889,7 +4943,7 @@
     </row>
     <row r="146" spans="1:10" ht="16" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="13"/>
-      <c r="B146" s="16"/>
+      <c r="B146" s="15"/>
       <c r="C146" s="6"/>
       <c r="D146" s="4"/>
       <c r="E146" s="4"/>
@@ -4900,7 +4954,7 @@
       <c r="J146" s="4"/>
     </row>
     <row r="147" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B147" s="16"/>
+      <c r="B147" s="15"/>
       <c r="C147" s="6"/>
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
@@ -4911,7 +4965,7 @@
       <c r="J147" s="4"/>
     </row>
     <row r="148" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B148" s="15"/>
+      <c r="B148" s="16"/>
       <c r="C148" s="6"/>
       <c r="D148" s="4"/>
       <c r="E148" s="4"/>
@@ -4935,7 +4989,7 @@
       <c r="J149" s="4"/>
     </row>
     <row r="150" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B150" s="16"/>
+      <c r="B150" s="15"/>
       <c r="C150" s="6"/>
       <c r="D150" s="4"/>
       <c r="E150" s="4"/>
@@ -4946,7 +5000,7 @@
       <c r="J150" s="4"/>
     </row>
     <row r="151" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B151" s="15"/>
+      <c r="B151" s="16"/>
       <c r="C151" s="6"/>
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
@@ -4983,7 +5037,7 @@
       <c r="J153" s="4"/>
     </row>
     <row r="154" spans="1:10" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B154" s="15"/>
+      <c r="B154" s="16"/>
       <c r="C154" s="6"/>
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
@@ -4996,6 +5050,13 @@
     <row r="155" spans="1:10" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B153:B154"/>
+    <mergeCell ref="B75:B82"/>
+    <mergeCell ref="B83:B87"/>
+    <mergeCell ref="B88:B102"/>
+    <mergeCell ref="B103:B119"/>
+    <mergeCell ref="B120:B138"/>
+    <mergeCell ref="B149:B151"/>
     <mergeCell ref="A131:A146"/>
     <mergeCell ref="B6:B13"/>
     <mergeCell ref="B14:B19"/>
@@ -5008,13 +5069,6 @@
     <mergeCell ref="B142:B144"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B145:B148"/>
-    <mergeCell ref="B153:B154"/>
-    <mergeCell ref="B75:B82"/>
-    <mergeCell ref="B83:B87"/>
-    <mergeCell ref="B88:B102"/>
-    <mergeCell ref="B103:B119"/>
-    <mergeCell ref="B120:B138"/>
-    <mergeCell ref="B149:B151"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>